<commit_message>
improved error handling and tracking especially with regards to CFL stability condition (if it isn't satified model stops that run)
</commit_message>
<xml_diff>
--- a/data/runtime-tracker.xlsx
+++ b/data/runtime-tracker.xlsx
@@ -14,13 +14,12 @@
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="regression" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet13" sheetId="17" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">regression!$O$3</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">regression!$P$3</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="53">
   <si>
     <t>run.n</t>
   </si>
@@ -187,12 +186,15 @@
   <si>
     <t>log(y)</t>
   </si>
+  <si>
+    <t>predict</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,8 +337,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -514,6 +523,24 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -697,7 +724,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -708,9 +735,11 @@
       <alignment horizontal="centerContinuous"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -784,6 +813,36 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mj-ea"/>
+                <a:cs typeface="+mj-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Model</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Run Time</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -798,16 +857,16 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mj-ea"/>
+              <a:cs typeface="+mj-cs"/>
             </a:defRPr>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
@@ -825,43 +884,45 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>regression!$G$1</c:f>
+              <c:f>regression!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>predict.run.time</c:v>
+                  <c:v>predict</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="flat" cmpd="dbl" algn="ctr">
               <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:symbol val="x"/>
+            <c:size val="6"/>
             <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
+              <a:noFill/>
+              <a:ln w="34925" cap="flat" cmpd="dbl" algn="ctr">
                 <a:solidFill>
-                  <a:schemeClr val="accent1"/>
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="75000"/>
+                    <a:alpha val="70000"/>
+                  </a:schemeClr>
                 </a:solidFill>
+                <a:round/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>regression!$A$2:$A$20</c:f>
+              <c:f>regression!$A$2:$A$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
                   <c:v>139.16999999999999</c:v>
                 </c:pt>
@@ -878,112 +939,214 @@
                   <c:v>5.27</c:v>
                 </c:pt>
                 <c:pt idx="5">
+                  <c:v>4.05</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.52</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.52</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.44</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.69</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3.34</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.36</c:v>
+                </c:pt>
+                <c:pt idx="14">
                   <c:v>88.24</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="15">
                   <c:v>72.930000000000007</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="16">
                   <c:v>65.73</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="17">
                   <c:v>24.57</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="18">
                   <c:v>22.46</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="19">
                   <c:v>20.260000000000002</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="20">
+                  <c:v>8.2899999999999991</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.37</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.87</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>88.38</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="24">
                   <c:v>73.42</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="25">
                   <c:v>64.739999999999995</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="26">
                   <c:v>25.57</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="27">
                   <c:v>21.89</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="28">
                   <c:v>20.190000000000001</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="29">
+                  <c:v>7.83</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>7.25</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>6.61</c:v>
+                </c:pt>
+                <c:pt idx="32">
                   <c:v>72.540000000000006</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="33">
                   <c:v>61.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>31.69</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>32.35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>regression!$G$2:$G$20</c:f>
+              <c:f>regression!$I$2:$I$37</c:f>
               <c:numCache>
-                <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="19"/>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="36"/>
                 <c:pt idx="0">
-                  <c:v>4.9345706972196695</c:v>
+                  <c:v>140.09412725462218</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9345706972196695</c:v>
+                  <c:v>140.09412725462218</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.9271865067093632</c:v>
+                  <c:v>139.23305334816868</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.9271865067093632</c:v>
+                  <c:v>139.23305334816868</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.6620303625532689</c:v>
+                  <c:v>5.5631328841104395</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.4488890251025879</c:v>
+                  <c:v>5.0353517252081419</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.3172317173559716</c:v>
+                  <c:v>1.9105327159404573</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.1855744096093543</c:v>
+                  <c:v>1.7292781617269739</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.2407486023843717</c:v>
+                  <c:v>0.20395527733606147</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.1090912946377554</c:v>
+                  <c:v>3.1548725107447679</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.9774339868911381</c:v>
+                  <c:v>2.8555659321322522</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.4488890251025879</c:v>
+                  <c:v>4.5670606967711276</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.3172317173559716</c:v>
+                  <c:v>4.1337781134620588</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.1855744096093543</c:v>
+                  <c:v>1.4196530068094455</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3.2407486023843717</c:v>
+                  <c:v>55.937295536576677</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3.1090912946377554</c:v>
+                  <c:v>50.630456516340807</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.9774339868911381</c:v>
+                  <c:v>45.827083745528483</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4.26576110044698</c:v>
+                  <c:v>32.780757703745294</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4.1341037927003637</c:v>
+                  <c:v>29.670807492059026</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26.855902026030435</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>11.257813061630124</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10.189770692672285</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>9.2230547976614119</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>55.937295536576677</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>50.630456516340807</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>45.827083745528483</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>32.780757703745294</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>29.670807492059026</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>26.855902026030435</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>11.257813061630124</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10.189770692672285</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>9.2230547976614119</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>48.006208957801142</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>43.451801733299703</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>23.31003734379734</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>23.31003734379734</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1027,20 +1190,88 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Actual </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" cap="none" baseline="0"/>
+                  <a:t>(min)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1089,20 +1320,88 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Predicted </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" cap="none" baseline="0"/>
+                  <a:t>(min)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1147,12 +1446,7 @@
       <a:schemeClr val="bg1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
+      <a:noFill/>
       <a:round/>
     </a:ln>
     <a:effectLst/>
@@ -1216,7 +1510,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="243">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1227,7 +1521,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1243,21 +1537,24 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="0" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1273,7 +1570,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1293,22 +1590,17 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
     <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
@@ -1317,37 +1609,49 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="25400" cap="flat" cmpd="dbl" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
@@ -1357,22 +1661,26 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525">
+      <a:ln w="34925" cap="flat" cmpd="dbl" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+            <a:alpha val="70000"/>
+          </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
@@ -1402,15 +1710,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1420,7 +1726,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1429,14 +1735,13 @@
           <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -1445,17 +1750,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1464,14 +1769,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1483,21 +1788,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1516,7 +1815,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1535,17 +1834,17 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="50000"/>
             <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
+        <a:prstDash val="dash"/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1554,17 +1853,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1585,7 +1883,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -1593,7 +1891,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1606,6 +1904,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1613,10 +1922,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -1631,17 +1940,17 @@
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
+    <cs:fontRef idx="major">
       <a:schemeClr val="tx1">
         <a:lumMod val="65000"/>
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="2000" kern="1200" spc="0" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
+      <cs:styleClr val="0"/>
     </cs:lnRef>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1649,11 +1958,14 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="38100" cap="rnd" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="phClr"/>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="75000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1674,20 +1986,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -1701,32 +2012,15 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="0" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -1735,16 +2029,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2029,10 +2323,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X35"/>
+  <dimension ref="A1:X37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2217,7 +2511,7 @@
         <v>7</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K35" si="1">C3*J3*I3/F3/B3</f>
+        <f t="shared" ref="K3:K37" si="1">C3*J3*I3/F3/B3</f>
         <v>0.20533333333333334</v>
       </c>
       <c r="L3">
@@ -4655,6 +4949,108 @@
       </c>
       <c r="X35">
         <v>3.7585894347103001E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>12.5</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>33.5</v>
+      </c>
+      <c r="E36">
+        <v>33.5</v>
+      </c>
+      <c r="F36">
+        <v>30</v>
+      </c>
+      <c r="G36">
+        <v>10</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+      <c r="I36">
+        <v>1.7</v>
+      </c>
+      <c r="J36">
+        <v>3</v>
+      </c>
+      <c r="K36">
+        <f t="shared" si="1"/>
+        <v>2.7199999999999998E-2</v>
+      </c>
+      <c r="L36">
+        <v>31.69</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36" t="s">
+        <v>22</v>
+      </c>
+      <c r="P36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37">
+        <v>12.5</v>
+      </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
+      <c r="D37">
+        <v>33.5</v>
+      </c>
+      <c r="E37">
+        <v>33.5</v>
+      </c>
+      <c r="F37">
+        <v>30</v>
+      </c>
+      <c r="G37">
+        <v>10</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37">
+        <v>1.7</v>
+      </c>
+      <c r="J37">
+        <v>3</v>
+      </c>
+      <c r="K37">
+        <f t="shared" si="1"/>
+        <v>2.7199999999999998E-2</v>
+      </c>
+      <c r="L37">
+        <v>32.35</v>
+      </c>
+      <c r="M37">
+        <v>0</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37" t="s">
+        <v>22</v>
+      </c>
+      <c r="P37">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -4664,10 +5060,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:H20"/>
+      <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4678,13 +5074,14 @@
     <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="5" customWidth="1"/>
+    <col min="10" max="10" width="7.85546875" style="5" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B1" t="str">
@@ -4707,15 +5104,18 @@
         <f>data!J1</f>
         <v>n.days</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="G1" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="9" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="I1" s="10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="8">
         <f>data!L2</f>
         <v>139.16999999999999</v>
       </c>
@@ -4739,24 +5139,24 @@
         <f>data!J2</f>
         <v>7</v>
       </c>
-      <c r="G2" s="6">
-        <f>regression!$K$18+regression!$K$19*B2+$K$20*C2+$K$21*D2+$K$22*E2+$K$23*F2</f>
-        <v>4.9345706972196695</v>
-      </c>
-      <c r="H2">
+      <c r="G2" s="7">
+        <f>regression!$L$18+regression!$L$19*B2+$L$20*C2+$L$21*D2+$L$22*E2+$L$23*F2</f>
+        <v>4.942314534224697</v>
+      </c>
+      <c r="H2" s="9">
         <f>LN(A2)</f>
         <v>4.9356962074317616</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="10">
         <f>EXP(G2)</f>
-        <v>139.01345085913746</v>
-      </c>
-      <c r="J2" t="s">
+        <v>140.09412725462218</v>
+      </c>
+      <c r="K2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="8">
         <f>data!L3</f>
         <v>139.04</v>
       </c>
@@ -4780,21 +5180,21 @@
         <f>data!J3</f>
         <v>7</v>
       </c>
-      <c r="G3" s="6">
-        <f>regression!$K$18+regression!$K$19*B3+$K$20*C3+$K$21*D3+$K$22*E3+$K$23*F3</f>
-        <v>4.9345706972196695</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H20" si="0">LN(A3)</f>
+      <c r="G3" s="7">
+        <f>regression!$L$18+regression!$L$19*B3+$L$20*C3+$L$21*D3+$L$22*E3+$L$23*F3</f>
+        <v>4.942314534224697</v>
+      </c>
+      <c r="H3" s="9">
+        <f t="shared" ref="H3:H37" si="0">LN(A3)</f>
         <v>4.934761661517082</v>
       </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I23" si="1">EXP(G3)</f>
-        <v>139.01345085913746</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
+      <c r="I3" s="10">
+        <f t="shared" ref="I3:I37" si="1">EXP(G3)</f>
+        <v>140.09412725462218</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <f>data!L4</f>
         <v>137.76</v>
       </c>
@@ -4818,25 +5218,25 @@
         <f>data!J4</f>
         <v>7</v>
       </c>
-      <c r="G4" s="6">
-        <f>regression!$K$18+regression!$K$19*B4+$K$20*C4+$K$21*D4+$K$22*E4+$K$23*F4</f>
-        <v>4.9271865067093632</v>
-      </c>
-      <c r="H4">
+      <c r="G4" s="7">
+        <f>regression!$L$18+regression!$L$19*B4+$L$20*C4+$L$21*D4+$L$22*E4+$L$23*F4</f>
+        <v>4.9361491719268598</v>
+      </c>
+      <c r="H4" s="9">
         <f t="shared" si="0"/>
         <v>4.9255130406794203</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="10">
         <f t="shared" si="1"/>
-        <v>137.99072968558403</v>
-      </c>
-      <c r="J4" s="4" t="s">
+        <v>139.23305334816868</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="L4" s="4"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
         <f>data!L5</f>
         <v>138.04</v>
       </c>
@@ -4860,27 +5260,27 @@
         <f>data!J5</f>
         <v>7</v>
       </c>
-      <c r="G5" s="6">
-        <f>regression!$K$18+regression!$K$19*B5+$K$20*C5+$K$21*D5+$K$22*E5+$K$23*F5</f>
-        <v>4.9271865067093632</v>
-      </c>
-      <c r="H5">
+      <c r="G5" s="7">
+        <f>regression!$L$18+regression!$L$19*B5+$L$20*C5+$L$21*D5+$L$22*E5+$L$23*F5</f>
+        <v>4.9361491719268598</v>
+      </c>
+      <c r="H5" s="9">
         <f t="shared" si="0"/>
         <v>4.9275434982298023</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="10">
         <f t="shared" si="1"/>
-        <v>137.99072968558403</v>
-      </c>
-      <c r="J5" s="1" t="s">
+        <v>139.23305334816868</v>
+      </c>
+      <c r="K5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="1">
-        <v>0.99972242574904402</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="L5" s="1">
+        <v>0.97261847018992109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <f>data!L6</f>
         <v>5.27</v>
       </c>
@@ -4904,942 +5304,1473 @@
         <f>data!J6</f>
         <v>1</v>
       </c>
-      <c r="G6" s="6">
-        <f>regression!$K$18+regression!$K$19*B6+$K$20*C6+$K$21*D6+$K$22*E6+$K$23*F6</f>
-        <v>1.6620303625532689</v>
-      </c>
-      <c r="H6">
+      <c r="G6" s="7">
+        <f>regression!$L$18+regression!$L$19*B6+$L$20*C6+$L$21*D6+$L$22*E6+$L$23*F6</f>
+        <v>1.7161614179389866</v>
+      </c>
+      <c r="H6" s="9">
         <f t="shared" si="0"/>
         <v>1.6620303625532709</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="10">
         <f t="shared" si="1"/>
-        <v>5.2699999999999889</v>
-      </c>
-      <c r="J6" s="1" t="s">
+        <v>5.5631328841104395</v>
+      </c>
+      <c r="K6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K6" s="1">
-        <v>0.99944492854555278</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+      <c r="L6" s="1">
+        <v>0.94598668855458246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <f>data!L7</f>
+        <v>4.05</v>
+      </c>
+      <c r="B7">
+        <f>data!B7</f>
+        <v>12.5</v>
+      </c>
+      <c r="C7">
+        <f>data!C7</f>
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <f>data!F7</f>
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <f>data!I7</f>
+        <v>2.8</v>
+      </c>
+      <c r="F7">
+        <f>data!J7</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="7">
+        <f>regression!$L$18+regression!$L$19*B7+$L$20*C7+$L$21*D7+$L$22*E7+$L$23*F7</f>
+        <v>1.6164833797799889</v>
+      </c>
+      <c r="H7" s="9">
+        <f t="shared" si="0"/>
+        <v>1.3987168811184478</v>
+      </c>
+      <c r="I7" s="10">
+        <f t="shared" si="1"/>
+        <v>5.0353517252081419</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0.93698446998034635</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <f>data!L8</f>
+        <v>1.7</v>
+      </c>
+      <c r="B8">
+        <f>data!B8</f>
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <f>data!C8</f>
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <f>data!F8</f>
+        <v>60</v>
+      </c>
+      <c r="E8">
+        <f>data!I8</f>
+        <v>2.8</v>
+      </c>
+      <c r="F8">
+        <f>data!J8</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="7">
+        <f>regression!$L$18+regression!$L$19*B8+$L$20*C8+$L$21*D8+$L$22*E8+$L$23*F8</f>
+        <v>0.64738211204003981</v>
+      </c>
+      <c r="H8" s="9">
+        <f t="shared" si="0"/>
+        <v>0.53062825106217038</v>
+      </c>
+      <c r="I8" s="10">
+        <f t="shared" si="1"/>
+        <v>1.9105327159404573</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0.38698028584063138</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="8">
+        <f>data!L9</f>
+        <v>1.52</v>
+      </c>
+      <c r="B9">
+        <f>data!B9</f>
+        <v>12.5</v>
+      </c>
+      <c r="C9">
+        <f>data!C9</f>
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <f>data!F9</f>
+        <v>60</v>
+      </c>
+      <c r="E9">
+        <f>data!I9</f>
+        <v>2.8</v>
+      </c>
+      <c r="F9">
+        <f>data!J9</f>
+        <v>1</v>
+      </c>
+      <c r="G9" s="7">
+        <f>regression!$L$18+regression!$L$19*B9+$L$20*C9+$L$21*D9+$L$22*E9+$L$23*F9</f>
+        <v>0.54770407388104214</v>
+      </c>
+      <c r="H9" s="9">
+        <f t="shared" si="0"/>
+        <v>0.41871033485818504</v>
+      </c>
+      <c r="I9" s="10">
+        <f t="shared" si="1"/>
+        <v>1.7292781617269739</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L9" s="2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <f>data!L10</f>
+        <v>0.75</v>
+      </c>
+      <c r="B10">
+        <f>data!B10</f>
+        <v>12.5</v>
+      </c>
+      <c r="C10">
+        <f>data!C10</f>
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <f>data!F10</f>
+        <v>120</v>
+      </c>
+      <c r="E10">
+        <f>data!I10</f>
+        <v>2.8</v>
+      </c>
+      <c r="F10">
+        <f>data!J10</f>
+        <v>1</v>
+      </c>
+      <c r="G10" s="7">
+        <f>regression!$L$18+regression!$L$19*B10+$L$20*C10+$L$21*D10+$L$22*E10+$L$23*F10</f>
+        <v>-1.5898545379168514</v>
+      </c>
+      <c r="H10" s="9">
+        <f t="shared" si="0"/>
+        <v>-0.2876820724517809</v>
+      </c>
+      <c r="I10" s="10">
+        <f t="shared" si="1"/>
+        <v>0.20395527733606147</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="8">
+        <f>data!L11</f>
+        <v>2.52</v>
+      </c>
+      <c r="B11">
+        <f>data!B11</f>
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <f>data!C11</f>
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f>data!F11</f>
+        <v>30</v>
+      </c>
+      <c r="E11">
+        <f>data!I11</f>
+        <v>0.5</v>
+      </c>
+      <c r="F11">
+        <f>data!J11</f>
+        <v>1</v>
+      </c>
+      <c r="G11" s="7">
+        <f>regression!$L$18+regression!$L$19*B11+$L$20*C11+$L$21*D11+$L$22*E11+$L$23*F11</f>
+        <v>1.1489480865379831</v>
+      </c>
+      <c r="H11" s="9">
+        <f t="shared" si="0"/>
+        <v>0.9242589015233319</v>
+      </c>
+      <c r="I11" s="10">
+        <f t="shared" si="1"/>
+        <v>3.1548725107447679</v>
+      </c>
+      <c r="K11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <f>data!L12</f>
+        <v>2.44</v>
+      </c>
+      <c r="B12">
+        <f>data!B12</f>
+        <v>12.5</v>
+      </c>
+      <c r="C12">
+        <f>data!C12</f>
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <f>data!F12</f>
+        <v>30</v>
+      </c>
+      <c r="E12">
+        <f>data!I12</f>
+        <v>0.5</v>
+      </c>
+      <c r="F12">
+        <f>data!J12</f>
+        <v>1</v>
+      </c>
+      <c r="G12" s="7">
+        <f>regression!$L$18+regression!$L$19*B12+$L$20*C12+$L$21*D12+$L$22*E12+$L$23*F12</f>
+        <v>1.0492700483789854</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" si="0"/>
+        <v>0.89199803930511046</v>
+      </c>
+      <c r="I12" s="10">
+        <f t="shared" si="1"/>
+        <v>2.8555659321322522</v>
+      </c>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <f>data!L13</f>
+        <v>3.69</v>
+      </c>
+      <c r="B13">
+        <f>data!B13</f>
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <f>data!C13</f>
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <f>data!F13</f>
+        <v>30</v>
+      </c>
+      <c r="E13">
+        <f>data!I13</f>
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <f>data!J13</f>
+        <v>1</v>
+      </c>
+      <c r="G13" s="7">
+        <f>regression!$L$18+regression!$L$19*B13+$L$20*C13+$L$21*D13+$L$22*E13+$L$23*F13</f>
+        <v>1.5188698244082028</v>
+      </c>
+      <c r="H13" s="9">
+        <f t="shared" si="0"/>
+        <v>1.3056264580524357</v>
+      </c>
+      <c r="I13" s="10">
+        <f t="shared" si="1"/>
+        <v>4.5670606967711276</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L13" s="1">
+        <v>5</v>
+      </c>
+      <c r="M13" s="1">
+        <v>78.683407303613336</v>
+      </c>
+      <c r="N13" s="1">
+        <v>15.736681460722668</v>
+      </c>
+      <c r="O13" s="1">
+        <v>105.0837280558742</v>
+      </c>
+      <c r="P13" s="1">
+        <v>4.4276915404545578E-18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <f>data!L14</f>
+        <v>3.34</v>
+      </c>
+      <c r="B14">
+        <f>data!B14</f>
+        <v>12.5</v>
+      </c>
+      <c r="C14">
+        <f>data!C14</f>
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <f>data!F14</f>
+        <v>30</v>
+      </c>
+      <c r="E14">
+        <f>data!I14</f>
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <f>data!J14</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="7">
+        <f>regression!$L$18+regression!$L$19*B14+$L$20*C14+$L$21*D14+$L$22*E14+$L$23*F14</f>
+        <v>1.4191917862492052</v>
+      </c>
+      <c r="H14" s="9">
+        <f t="shared" si="0"/>
+        <v>1.205970806988609</v>
+      </c>
+      <c r="I14" s="10">
+        <f t="shared" si="1"/>
+        <v>4.1337781134620588</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="1">
+        <v>30</v>
+      </c>
+      <c r="M14" s="1">
+        <v>4.4926122488789026</v>
+      </c>
+      <c r="N14" s="1">
+        <v>0.14975374162929675</v>
+      </c>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="8">
+        <f>data!L15</f>
+        <v>1.36</v>
+      </c>
+      <c r="B15">
+        <f>data!B15</f>
+        <v>12.5</v>
+      </c>
+      <c r="C15">
+        <f>data!C15</f>
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <f>data!F15</f>
+        <v>60</v>
+      </c>
+      <c r="E15">
+        <f>data!I15</f>
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <f>data!J15</f>
+        <v>1</v>
+      </c>
+      <c r="G15" s="7">
+        <f>regression!$L$18+regression!$L$19*B15+$L$20*C15+$L$21*D15+$L$22*E15+$L$23*F15</f>
+        <v>0.3504124803502584</v>
+      </c>
+      <c r="H15" s="9">
+        <f t="shared" si="0"/>
+        <v>0.30748469974796072</v>
+      </c>
+      <c r="I15" s="10">
+        <f t="shared" si="1"/>
+        <v>1.4196530068094455</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="L15" s="2">
+        <v>35</v>
+      </c>
+      <c r="M15" s="2">
+        <v>83.176019552492235</v>
+      </c>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="2"/>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="8">
         <f>data!L16</f>
         <v>88.24</v>
       </c>
-      <c r="B7">
+      <c r="B16">
         <f>data!B16</f>
         <v>10</v>
       </c>
-      <c r="C7">
+      <c r="C16">
         <f>data!C16</f>
         <v>1</v>
       </c>
-      <c r="D7">
+      <c r="D16">
         <f>data!F16</f>
         <v>15</v>
       </c>
-      <c r="E7">
+      <c r="E16">
         <f>data!I16</f>
         <v>3</v>
       </c>
-      <c r="F7">
+      <c r="F16">
         <f>data!J16</f>
         <v>3</v>
       </c>
-      <c r="G7" s="6">
-        <f>regression!$K$18+regression!$K$19*B7+$K$20*C7+$K$21*D7+$K$22*E7+$K$23*F7</f>
-        <v>4.4488890251025879</v>
-      </c>
-      <c r="H7">
+      <c r="G16" s="7">
+        <f>regression!$L$18+regression!$L$19*B16+$L$20*C16+$L$21*D16+$L$22*E16+$L$23*F16</f>
+        <v>4.0242313408163568</v>
+      </c>
+      <c r="H16" s="9">
         <f t="shared" si="0"/>
         <v>4.4800603749452472</v>
       </c>
-      <c r="I7">
+      <c r="I16" s="10">
         <f t="shared" si="1"/>
-        <v>85.531867440487858</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0.99923143952461158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
+        <v>55.937295536576677</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
         <f>data!L17</f>
         <v>72.930000000000007</v>
       </c>
-      <c r="B8">
+      <c r="B17">
         <f>data!B17</f>
         <v>12.5</v>
       </c>
-      <c r="C8">
+      <c r="C17">
         <f>data!C17</f>
         <v>1</v>
       </c>
-      <c r="D8">
+      <c r="D17">
         <f>data!F17</f>
         <v>15</v>
       </c>
-      <c r="E8">
+      <c r="E17">
         <f>data!I17</f>
         <v>3</v>
       </c>
-      <c r="F8">
+      <c r="F17">
         <f>data!J17</f>
         <v>3</v>
       </c>
-      <c r="G8" s="6">
-        <f>regression!$K$18+regression!$K$19*B8+$K$20*C8+$K$21*D8+$K$22*E8+$K$23*F8</f>
-        <v>4.3172317173559716</v>
-      </c>
-      <c r="H8">
+      <c r="G17" s="7">
+        <f>regression!$L$18+regression!$L$19*B17+$L$20*C17+$L$21*D17+$L$22*E17+$L$23*F17</f>
+        <v>3.9245533026573596</v>
+      </c>
+      <c r="H17" s="9">
         <f t="shared" si="0"/>
         <v>4.2895000769961422</v>
       </c>
-      <c r="I8">
+      <c r="I17" s="10">
         <f t="shared" si="1"/>
-        <v>74.980772751476451</v>
-      </c>
-      <c r="J8" s="1" t="s">
+        <v>50.630456516340807</v>
+      </c>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M17" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="K8" s="1">
-        <v>2.4786873972058327E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="5">
+      <c r="N17" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="P17" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="R17" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="S17" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
         <f>data!L18</f>
         <v>65.73</v>
       </c>
-      <c r="B9">
+      <c r="B18">
         <f>data!B18</f>
         <v>15</v>
       </c>
-      <c r="C9">
+      <c r="C18">
         <f>data!C18</f>
         <v>1</v>
       </c>
-      <c r="D9">
+      <c r="D18">
         <f>data!F18</f>
         <v>15</v>
       </c>
-      <c r="E9">
+      <c r="E18">
         <f>data!I18</f>
         <v>3</v>
       </c>
-      <c r="F9">
+      <c r="F18">
         <f>data!J18</f>
         <v>3</v>
       </c>
-      <c r="G9" s="6">
-        <f>regression!$K$18+regression!$K$19*B9+$K$20*C9+$K$21*D9+$K$22*E9+$K$23*F9</f>
-        <v>4.1855744096093543</v>
-      </c>
-      <c r="H9">
+      <c r="G18" s="7">
+        <f>regression!$L$18+regression!$L$19*B18+$L$20*C18+$L$21*D18+$L$22*E18+$L$23*F18</f>
+        <v>3.8248752644983619</v>
+      </c>
+      <c r="H18" s="9">
         <f t="shared" si="0"/>
         <v>4.1855554422754846</v>
       </c>
-      <c r="I9">
+      <c r="I18" s="10">
         <f t="shared" si="1"/>
-        <v>65.73124673467882</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K9" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
+        <v>45.827083745528483</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="L18" s="1">
+        <v>1.5516343684670519</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0.51201095089277793</v>
+      </c>
+      <c r="N18" s="1">
+        <v>3.0304710587957429</v>
+      </c>
+      <c r="O18" s="1">
+        <v>4.9915117869967374E-3</v>
+      </c>
+      <c r="P18" s="1">
+        <v>0.50596850613412592</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>2.597300230799978</v>
+      </c>
+      <c r="R18" s="1">
+        <v>0.50596850613412592</v>
+      </c>
+      <c r="S18" s="1">
+        <v>2.597300230799978</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
         <f>data!L19</f>
         <v>24.57</v>
       </c>
-      <c r="B10">
+      <c r="B19">
         <f>data!B19</f>
         <v>10</v>
       </c>
-      <c r="C10">
+      <c r="C19">
         <f>data!C19</f>
         <v>1</v>
       </c>
-      <c r="D10">
+      <c r="D19">
         <f>data!F19</f>
         <v>30</v>
       </c>
-      <c r="E10">
+      <c r="E19">
         <f>data!I19</f>
         <v>3</v>
       </c>
-      <c r="F10">
+      <c r="F19">
         <f>data!J19</f>
         <v>3</v>
       </c>
-      <c r="G10" s="6">
-        <f>regression!$K$18+regression!$K$19*B10+$K$20*C10+$K$21*D10+$K$22*E10+$K$23*F10</f>
-        <v>3.2407486023843717</v>
-      </c>
-      <c r="H10">
+      <c r="G19" s="7">
+        <f>regression!$L$18+regression!$L$19*B19+$L$20*C19+$L$21*D19+$L$22*E19+$L$23*F19</f>
+        <v>3.4898416878668836</v>
+      </c>
+      <c r="H19" s="9">
         <f t="shared" si="0"/>
         <v>3.201526186533088</v>
       </c>
-      <c r="I10">
+      <c r="I19" s="10">
         <f t="shared" si="1"/>
-        <v>25.552843508738562</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
+        <v>32.780757703745294</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L19" s="1">
+        <v>-3.9871215263599068E-2</v>
+      </c>
+      <c r="M19" s="1">
+        <v>3.9796367470602924E-2</v>
+      </c>
+      <c r="N19" s="1">
+        <v>-1.0018807694710186</v>
+      </c>
+      <c r="O19" s="1">
+        <v>0.32441423601876773</v>
+      </c>
+      <c r="P19" s="1">
+        <v>-0.12114624040965397</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>4.1403809882455837E-2</v>
+      </c>
+      <c r="R19" s="1">
+        <v>-0.12114624040965397</v>
+      </c>
+      <c r="S19" s="1">
+        <v>4.1403809882455837E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
         <f>data!L20</f>
         <v>22.46</v>
       </c>
-      <c r="B11">
+      <c r="B20">
         <f>data!B20</f>
         <v>12.5</v>
       </c>
-      <c r="C11">
+      <c r="C20">
         <f>data!C20</f>
         <v>1</v>
       </c>
-      <c r="D11">
+      <c r="D20">
         <f>data!F20</f>
         <v>30</v>
       </c>
-      <c r="E11">
+      <c r="E20">
         <f>data!I20</f>
         <v>3</v>
       </c>
-      <c r="F11">
+      <c r="F20">
         <f>data!J20</f>
         <v>3</v>
       </c>
-      <c r="G11" s="6">
-        <f>regression!$K$18+regression!$K$19*B11+$K$20*C11+$K$21*D11+$K$22*E11+$K$23*F11</f>
-        <v>3.1090912946377554</v>
-      </c>
-      <c r="H11">
+      <c r="G20" s="7">
+        <f>regression!$L$18+regression!$L$19*B20+$L$20*C20+$L$21*D20+$L$22*E20+$L$23*F20</f>
+        <v>3.390163649707886</v>
+      </c>
+      <c r="H20" s="9">
         <f t="shared" si="0"/>
         <v>3.111735949310297</v>
       </c>
-      <c r="I11">
+      <c r="I20" s="10">
         <f t="shared" si="1"/>
-        <v>22.400679531706459</v>
-      </c>
-      <c r="J11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+        <v>29.670807492059026</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L20" s="1">
+        <v>7.9319244876528042E-2</v>
+      </c>
+      <c r="M20" s="1">
+        <v>3.736856582066992E-2</v>
+      </c>
+      <c r="N20" s="1">
+        <v>2.1226194566090002</v>
+      </c>
+      <c r="O20" s="1">
+        <v>4.215179425321277E-2</v>
+      </c>
+      <c r="P20" s="1">
+        <v>3.0024521694940048E-3</v>
+      </c>
+      <c r="Q20" s="1">
+        <v>0.15563603758356209</v>
+      </c>
+      <c r="R20" s="1">
+        <v>3.0024521694940048E-3</v>
+      </c>
+      <c r="S20" s="1">
+        <v>0.15563603758356209</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
         <f>data!L21</f>
         <v>20.260000000000002</v>
       </c>
-      <c r="B12">
+      <c r="B21">
         <f>data!B21</f>
         <v>15</v>
       </c>
-      <c r="C12">
+      <c r="C21">
         <f>data!C21</f>
         <v>1</v>
       </c>
-      <c r="D12">
+      <c r="D21">
         <f>data!F21</f>
         <v>30</v>
       </c>
-      <c r="E12">
+      <c r="E21">
         <f>data!I21</f>
         <v>3</v>
       </c>
-      <c r="F12">
+      <c r="F21">
         <f>data!J21</f>
         <v>3</v>
       </c>
-      <c r="G12" s="6">
-        <f>regression!$K$18+regression!$K$19*B12+$K$20*C12+$K$21*D12+$K$22*E12+$K$23*F12</f>
-        <v>2.9774339868911381</v>
-      </c>
-      <c r="H12">
+      <c r="G21" s="7">
+        <f>regression!$L$18+regression!$L$19*B21+$L$20*C21+$L$21*D21+$L$22*E21+$L$23*F21</f>
+        <v>3.2904856115488883</v>
+      </c>
+      <c r="H21" s="9">
         <f t="shared" si="0"/>
         <v>3.0086484988205373</v>
       </c>
-      <c r="I12">
+      <c r="I21" s="10">
         <f t="shared" si="1"/>
-        <v>19.637362210221731</v>
-      </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
+        <v>26.855902026030435</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L21" s="1">
+        <v>-3.5625976863298228E-2</v>
+      </c>
+      <c r="M21" s="1">
+        <v>3.4421403155828591E-3</v>
+      </c>
+      <c r="N21" s="1">
+        <v>-10.349949042465362</v>
+      </c>
+      <c r="O21" s="1">
+        <v>2.0412078251008695E-11</v>
+      </c>
+      <c r="P21" s="1">
+        <v>-4.2655765220537149E-2</v>
+      </c>
+      <c r="Q21" s="1">
+        <v>-2.8596188506059304E-2</v>
+      </c>
+      <c r="R21" s="1">
+        <v>-4.2655765220537149E-2</v>
+      </c>
+      <c r="S21" s="1">
+        <v>-2.8596188506059304E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <f>data!L22</f>
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="B22">
+        <f>data!B22</f>
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <f>data!C22</f>
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <f>data!F22</f>
+        <v>60</v>
+      </c>
+      <c r="E22">
+        <f>data!I22</f>
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <f>data!J22</f>
+        <v>3</v>
+      </c>
+      <c r="G22" s="7">
+        <f>regression!$L$18+regression!$L$19*B22+$L$20*C22+$L$21*D22+$L$22*E22+$L$23*F22</f>
+        <v>2.4210623819679369</v>
+      </c>
+      <c r="H22" s="9">
+        <f t="shared" si="0"/>
+        <v>2.1150499691472033</v>
+      </c>
+      <c r="I22" s="10">
+        <f t="shared" si="1"/>
+        <v>11.257813061630124</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L22" s="1">
+        <v>0.24661449191347981</v>
+      </c>
+      <c r="M22" s="1">
+        <v>0.12762708873809955</v>
+      </c>
+      <c r="N22" s="1">
+        <v>1.9323052367005833</v>
+      </c>
+      <c r="O22" s="1">
+        <v>6.2812973785318263E-2</v>
+      </c>
+      <c r="P22" s="1">
+        <v>-1.4034796094254814E-2</v>
+      </c>
+      <c r="Q22" s="1">
+        <v>0.50726377992121441</v>
+      </c>
+      <c r="R22" s="1">
+        <v>-1.4034796094254814E-2</v>
+      </c>
+      <c r="S22" s="1">
+        <v>0.50726377992121441</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="8">
+        <f>data!L23</f>
+        <v>7.37</v>
+      </c>
+      <c r="B23">
+        <f>data!B23</f>
+        <v>12.5</v>
+      </c>
+      <c r="C23">
+        <f>data!C23</f>
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <f>data!F23</f>
+        <v>60</v>
+      </c>
+      <c r="E23">
+        <f>data!I23</f>
+        <v>3</v>
+      </c>
+      <c r="F23">
+        <f>data!J23</f>
+        <v>3</v>
+      </c>
+      <c r="G23" s="7">
+        <f>regression!$L$18+regression!$L$19*B23+$L$20*C23+$L$21*D23+$L$22*E23+$L$23*F23</f>
+        <v>2.3213843438089392</v>
+      </c>
+      <c r="H23" s="9">
+        <f t="shared" si="0"/>
+        <v>1.9974177062012453</v>
+      </c>
+      <c r="I23" s="10">
+        <f t="shared" si="1"/>
+        <v>10.189770692672285</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0.86217868577260059</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0.10020322390775445</v>
+      </c>
+      <c r="N23" s="2">
+        <v>8.6043008612807608</v>
+      </c>
+      <c r="O23" s="2">
+        <v>1.3411484597455436E-9</v>
+      </c>
+      <c r="P23" s="2">
+        <v>0.65753640155320803</v>
+      </c>
+      <c r="Q23" s="2">
+        <v>1.0668209699919933</v>
+      </c>
+      <c r="R23" s="2">
+        <v>0.65753640155320803</v>
+      </c>
+      <c r="S23" s="2">
+        <v>1.0668209699919933</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <f>data!L24</f>
+        <v>6.87</v>
+      </c>
+      <c r="B24">
+        <f>data!B24</f>
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <f>data!C24</f>
+        <v>1</v>
+      </c>
+      <c r="D24">
+        <f>data!F24</f>
+        <v>60</v>
+      </c>
+      <c r="E24">
+        <f>data!I24</f>
+        <v>3</v>
+      </c>
+      <c r="F24">
+        <f>data!J24</f>
+        <v>3</v>
+      </c>
+      <c r="G24" s="7">
+        <f>regression!$L$18+regression!$L$19*B24+$L$20*C24+$L$21*D24+$L$22*E24+$L$23*F24</f>
+        <v>2.2217063056499415</v>
+      </c>
+      <c r="H24" s="9">
+        <f t="shared" si="0"/>
+        <v>1.9271641062342579</v>
+      </c>
+      <c r="I24" s="10">
+        <f t="shared" si="1"/>
+        <v>9.2230547976614119</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
         <f>data!L25</f>
         <v>88.38</v>
       </c>
-      <c r="B13">
+      <c r="B25">
         <f>data!B25</f>
         <v>10</v>
       </c>
-      <c r="C13">
+      <c r="C25">
         <f>data!C25</f>
         <v>1</v>
       </c>
-      <c r="D13">
+      <c r="D25">
         <f>data!F25</f>
         <v>15</v>
       </c>
-      <c r="E13">
+      <c r="E25">
         <f>data!I25</f>
         <v>3</v>
       </c>
-      <c r="F13">
+      <c r="F25">
         <f>data!J25</f>
         <v>3</v>
       </c>
-      <c r="G13" s="6">
-        <f>regression!$K$18+regression!$K$19*B13+$K$20*C13+$K$21*D13+$K$22*E13+$K$23*F13</f>
-        <v>4.4488890251025879</v>
-      </c>
-      <c r="H13">
+      <c r="G25" s="7">
+        <f>regression!$L$18+regression!$L$19*B25+$L$20*C25+$L$21*D25+$L$22*E25+$L$23*F25</f>
+        <v>4.0242313408163568</v>
+      </c>
+      <c r="H25" s="9">
         <f t="shared" si="0"/>
         <v>4.481645699702594</v>
       </c>
-      <c r="I13">
+      <c r="I25" s="10">
         <f t="shared" si="1"/>
-        <v>85.531867440487858</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="K13" s="1">
-        <v>5</v>
-      </c>
-      <c r="L13" s="1">
-        <v>14.381256908113283</v>
-      </c>
-      <c r="M13" s="1">
-        <v>2.8762513816226565</v>
-      </c>
-      <c r="N13" s="1">
-        <v>4681.4816243903415</v>
-      </c>
-      <c r="O13" s="1">
-        <v>1.1161070731717967E-20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
+        <v>55.937295536576677</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
         <f>data!L26</f>
         <v>73.42</v>
       </c>
-      <c r="B14">
+      <c r="B26">
         <f>data!B26</f>
         <v>12.5</v>
       </c>
-      <c r="C14">
+      <c r="C26">
         <f>data!C26</f>
         <v>1</v>
       </c>
-      <c r="D14">
+      <c r="D26">
         <f>data!F26</f>
         <v>15</v>
       </c>
-      <c r="E14">
+      <c r="E26">
         <f>data!I26</f>
         <v>3</v>
       </c>
-      <c r="F14">
+      <c r="F26">
         <f>data!J26</f>
         <v>3</v>
       </c>
-      <c r="G14" s="6">
-        <f>regression!$K$18+regression!$K$19*B14+$K$20*C14+$K$21*D14+$K$22*E14+$K$23*F14</f>
-        <v>4.3172317173559716</v>
-      </c>
-      <c r="H14">
+      <c r="G26" s="7">
+        <f>regression!$L$18+regression!$L$19*B26+$L$20*C26+$L$21*D26+$L$22*E26+$L$23*F26</f>
+        <v>3.9245533026573596</v>
+      </c>
+      <c r="H26" s="9">
         <f t="shared" si="0"/>
         <v>4.2961963780686885</v>
       </c>
-      <c r="I14">
+      <c r="I26" s="10">
         <f t="shared" si="1"/>
-        <v>74.980772751476451</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K14" s="1">
-        <v>13</v>
-      </c>
-      <c r="L14" s="1">
-        <v>7.9870585769871334E-3</v>
-      </c>
-      <c r="M14" s="1">
-        <v>6.1438912130670255E-4</v>
-      </c>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="5">
+        <v>50.630456516340807</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
         <f>data!L27</f>
         <v>64.739999999999995</v>
       </c>
-      <c r="B15">
+      <c r="B27">
         <f>data!B27</f>
         <v>15</v>
       </c>
-      <c r="C15">
+      <c r="C27">
         <f>data!C27</f>
         <v>1</v>
       </c>
-      <c r="D15">
+      <c r="D27">
         <f>data!F27</f>
         <v>15</v>
       </c>
-      <c r="E15">
+      <c r="E27">
         <f>data!I27</f>
         <v>3</v>
       </c>
-      <c r="F15">
+      <c r="F27">
         <f>data!J27</f>
         <v>3</v>
       </c>
-      <c r="G15" s="6">
-        <f>regression!$K$18+regression!$K$19*B15+$K$20*C15+$K$21*D15+$K$22*E15+$K$23*F15</f>
-        <v>4.1855744096093543</v>
-      </c>
-      <c r="H15">
+      <c r="G27" s="7">
+        <f>regression!$L$18+regression!$L$19*B27+$L$20*C27+$L$21*D27+$L$22*E27+$L$23*F27</f>
+        <v>3.8248752644983619</v>
+      </c>
+      <c r="H27" s="9">
         <f t="shared" si="0"/>
         <v>4.1703792484980982</v>
       </c>
-      <c r="I15">
+      <c r="I27" s="10">
         <f t="shared" si="1"/>
-        <v>65.73124673467882</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="K15" s="2">
-        <v>18</v>
-      </c>
-      <c r="L15" s="2">
-        <v>14.38924396669027</v>
-      </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-    </row>
-    <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="5">
+        <v>45.827083745528483</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
         <f>data!L28</f>
         <v>25.57</v>
       </c>
-      <c r="B16">
+      <c r="B28">
         <f>data!B28</f>
         <v>10</v>
       </c>
-      <c r="C16">
+      <c r="C28">
         <f>data!C28</f>
         <v>1</v>
       </c>
-      <c r="D16">
+      <c r="D28">
         <f>data!F28</f>
         <v>30</v>
       </c>
-      <c r="E16">
+      <c r="E28">
         <f>data!I28</f>
         <v>3</v>
       </c>
-      <c r="F16">
+      <c r="F28">
         <f>data!J28</f>
         <v>3</v>
       </c>
-      <c r="G16" s="6">
-        <f>regression!$K$18+regression!$K$19*B16+$K$20*C16+$K$21*D16+$K$22*E16+$K$23*F16</f>
-        <v>3.2407486023843717</v>
-      </c>
-      <c r="H16">
+      <c r="G28" s="7">
+        <f>regression!$L$18+regression!$L$19*B28+$L$20*C28+$L$21*D28+$L$22*E28+$L$23*F28</f>
+        <v>3.4898416878668836</v>
+      </c>
+      <c r="H28" s="9">
         <f t="shared" si="0"/>
         <v>3.2414197893030954</v>
       </c>
-      <c r="I16">
+      <c r="I28" s="10">
         <f t="shared" si="1"/>
-        <v>25.552843508738562</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+        <v>32.780757703745294</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
         <f>data!L29</f>
         <v>21.89</v>
       </c>
-      <c r="B17">
+      <c r="B29">
         <f>data!B29</f>
         <v>12.5</v>
       </c>
-      <c r="C17">
+      <c r="C29">
         <f>data!C29</f>
         <v>1</v>
       </c>
-      <c r="D17">
+      <c r="D29">
         <f>data!F29</f>
         <v>30</v>
       </c>
-      <c r="E17">
+      <c r="E29">
         <f>data!I29</f>
         <v>3</v>
       </c>
-      <c r="F17">
+      <c r="F29">
         <f>data!J29</f>
         <v>3</v>
       </c>
-      <c r="G17" s="6">
-        <f>regression!$K$18+regression!$K$19*B17+$K$20*C17+$K$21*D17+$K$22*E17+$K$23*F17</f>
-        <v>3.1090912946377554</v>
-      </c>
-      <c r="H17">
+      <c r="G29" s="7">
+        <f>regression!$L$18+regression!$L$19*B29+$L$20*C29+$L$21*D29+$L$22*E29+$L$23*F29</f>
+        <v>3.390163649707886</v>
+      </c>
+      <c r="H29" s="9">
         <f t="shared" si="0"/>
         <v>3.0860299115347716</v>
       </c>
-      <c r="I17">
+      <c r="I29" s="10">
         <f t="shared" si="1"/>
-        <v>22.400679531706459</v>
-      </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="L17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="N17" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="O17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="P17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
+        <v>29.670807492059026</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
         <f>data!L30</f>
         <v>20.190000000000001</v>
       </c>
-      <c r="B18">
+      <c r="B30">
         <f>data!B30</f>
         <v>15</v>
       </c>
-      <c r="C18">
+      <c r="C30">
         <f>data!C30</f>
         <v>1</v>
       </c>
-      <c r="D18">
+      <c r="D30">
         <f>data!F30</f>
         <v>30</v>
       </c>
-      <c r="E18">
+      <c r="E30">
         <f>data!I30</f>
         <v>3</v>
       </c>
-      <c r="F18">
+      <c r="F30">
         <f>data!J30</f>
         <v>3</v>
       </c>
-      <c r="G18" s="6">
-        <f>regression!$K$18+regression!$K$19*B18+$K$20*C18+$K$21*D18+$K$22*E18+$K$23*F18</f>
-        <v>2.9774339868911381</v>
-      </c>
-      <c r="H18">
+      <c r="G30" s="7">
+        <f>regression!$L$18+regression!$L$19*B30+$L$20*C30+$L$21*D30+$L$22*E30+$L$23*F30</f>
+        <v>3.2904856115488883</v>
+      </c>
+      <c r="H30" s="9">
         <f t="shared" si="0"/>
         <v>3.0051874323247461</v>
       </c>
-      <c r="I18">
+      <c r="I30" s="10">
         <f t="shared" si="1"/>
-        <v>19.637362210221731</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K18" s="1">
-        <v>2.6880189226988693</v>
-      </c>
-      <c r="L18" s="1">
-        <v>9.2942731268202947E-2</v>
-      </c>
-      <c r="M18" s="1">
-        <v>28.921238767366411</v>
-      </c>
-      <c r="N18" s="1">
-        <v>3.4737645764788193E-13</v>
-      </c>
-      <c r="O18" s="1">
-        <v>2.4872283592209992</v>
-      </c>
-      <c r="P18" s="1">
-        <v>2.8888094861767395</v>
-      </c>
-      <c r="Q18" s="1">
-        <v>2.4872283592209992</v>
-      </c>
-      <c r="R18" s="1">
-        <v>2.8888094861767395</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
+        <v>26.855902026030435</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <f>data!L31</f>
+        <v>7.83</v>
+      </c>
+      <c r="B31">
+        <f>data!B31</f>
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <f>data!C31</f>
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <f>data!F31</f>
+        <v>60</v>
+      </c>
+      <c r="E31">
+        <f>data!I31</f>
+        <v>3</v>
+      </c>
+      <c r="F31">
+        <f>data!J31</f>
+        <v>3</v>
+      </c>
+      <c r="G31" s="7">
+        <f>regression!$L$18+regression!$L$19*B31+$L$20*C31+$L$21*D31+$L$22*E31+$L$23*F31</f>
+        <v>2.4210623819679369</v>
+      </c>
+      <c r="H31" s="9">
+        <f t="shared" si="0"/>
+        <v>2.0579625100027119</v>
+      </c>
+      <c r="I31" s="10">
+        <f t="shared" si="1"/>
+        <v>11.257813061630124</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <f>data!L32</f>
+        <v>7.25</v>
+      </c>
+      <c r="B32">
+        <f>data!B32</f>
+        <v>12.5</v>
+      </c>
+      <c r="C32">
+        <f>data!C32</f>
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <f>data!F32</f>
+        <v>60</v>
+      </c>
+      <c r="E32">
+        <f>data!I32</f>
+        <v>3</v>
+      </c>
+      <c r="F32">
+        <f>data!J32</f>
+        <v>3</v>
+      </c>
+      <c r="G32" s="7">
+        <f>regression!$L$18+regression!$L$19*B32+$L$20*C32+$L$21*D32+$L$22*E32+$L$23*F32</f>
+        <v>2.3213843438089392</v>
+      </c>
+      <c r="H32" s="9">
+        <f t="shared" si="0"/>
+        <v>1.9810014688665833</v>
+      </c>
+      <c r="I32" s="10">
+        <f t="shared" si="1"/>
+        <v>10.189770692672285</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
+        <f>data!L33</f>
+        <v>6.61</v>
+      </c>
+      <c r="B33">
+        <f>data!B33</f>
+        <v>15</v>
+      </c>
+      <c r="C33">
+        <f>data!C33</f>
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <f>data!F33</f>
+        <v>60</v>
+      </c>
+      <c r="E33">
+        <f>data!I33</f>
+        <v>3</v>
+      </c>
+      <c r="F33">
+        <f>data!J33</f>
+        <v>3</v>
+      </c>
+      <c r="G33" s="7">
+        <f>regression!$L$18+regression!$L$19*B33+$L$20*C33+$L$21*D33+$L$22*E33+$L$23*F33</f>
+        <v>2.2217063056499415</v>
+      </c>
+      <c r="H33" s="9">
+        <f t="shared" si="0"/>
+        <v>1.8885836538635949</v>
+      </c>
+      <c r="I33" s="10">
+        <f t="shared" si="1"/>
+        <v>9.2230547976614119</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
         <f>data!L34</f>
         <v>72.540000000000006</v>
       </c>
-      <c r="B19">
+      <c r="B34">
         <f>data!B34</f>
         <v>10</v>
       </c>
-      <c r="C19">
+      <c r="C34">
         <f>data!C34</f>
         <v>1</v>
       </c>
-      <c r="D19">
+      <c r="D34">
         <f>data!F34</f>
         <v>15</v>
       </c>
-      <c r="E19">
+      <c r="E34">
         <f>data!I34</f>
         <v>2.38</v>
       </c>
-      <c r="F19">
+      <c r="F34">
         <f>data!J34</f>
         <v>3</v>
       </c>
-      <c r="G19" s="6">
-        <f>regression!$K$18+regression!$K$19*B19+$K$20*C19+$K$21*D19+$K$22*E19+$K$23*F19</f>
-        <v>4.26576110044698</v>
-      </c>
-      <c r="H19">
+      <c r="G34" s="7">
+        <f>regression!$L$18+regression!$L$19*B34+$L$20*C34+$L$21*D34+$L$22*E34+$L$23*F34</f>
+        <v>3.8713303558299996</v>
+      </c>
+      <c r="H34" s="9">
         <f t="shared" si="0"/>
         <v>4.2841381338547562</v>
       </c>
-      <c r="I19">
+      <c r="I34" s="10">
         <f t="shared" si="1"/>
-        <v>71.219104243016304</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K19" s="1">
-        <v>-5.266292309864673E-2</v>
-      </c>
-      <c r="L19" s="1">
-        <v>3.4006498309985759E-3</v>
-      </c>
-      <c r="M19" s="1">
-        <v>-15.486135214098962</v>
-      </c>
-      <c r="N19" s="1">
-        <v>9.3085819315437017E-10</v>
-      </c>
-      <c r="O19" s="1">
-        <v>-6.0009580405141545E-2</v>
-      </c>
-      <c r="P19" s="1">
-        <v>-4.5316265792151915E-2</v>
-      </c>
-      <c r="Q19" s="1">
-        <v>-6.0009580405141545E-2</v>
-      </c>
-      <c r="R19" s="1">
-        <v>-4.5316265792151915E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
+        <v>48.006208957801142</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
         <f>data!L35</f>
         <v>61.3</v>
       </c>
-      <c r="B20">
+      <c r="B35">
         <f>data!B35</f>
         <v>12.5</v>
       </c>
-      <c r="C20">
+      <c r="C35">
         <f>data!C35</f>
         <v>1</v>
       </c>
-      <c r="D20">
+      <c r="D35">
         <f>data!F35</f>
         <v>15</v>
       </c>
-      <c r="E20">
+      <c r="E35">
         <f>data!I35</f>
         <v>2.38</v>
       </c>
-      <c r="F20">
+      <c r="F35">
         <f>data!J35</f>
         <v>3</v>
       </c>
-      <c r="G20" s="6">
-        <f>regression!$K$18+regression!$K$19*B20+$K$20*C20+$K$21*D20+$K$22*E20+$K$23*F20</f>
-        <v>4.1341037927003637</v>
-      </c>
-      <c r="H20">
+      <c r="G35" s="7">
+        <f>regression!$L$18+regression!$L$19*B35+$L$20*C35+$L$21*D35+$L$22*E35+$L$23*F35</f>
+        <v>3.771652317671002</v>
+      </c>
+      <c r="H35" s="9">
         <f t="shared" si="0"/>
         <v>4.1157798429421657</v>
       </c>
-      <c r="I20">
+      <c r="I35" s="10">
         <f t="shared" si="1"/>
-        <v>62.433612530731622</v>
-      </c>
-      <c r="J20" s="1" t="s">
+        <v>43.451801733299703</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
+        <f>data!L36</f>
+        <v>31.69</v>
+      </c>
+      <c r="B36">
+        <f>data!B36</f>
+        <v>12.5</v>
+      </c>
+      <c r="C36">
+        <f>data!C36</f>
         <v>2</v>
       </c>
-      <c r="K20" s="1">
-        <v>0.33006982124861739</v>
-      </c>
-      <c r="L20" s="1">
-        <v>7.1841242965634431E-3</v>
-      </c>
-      <c r="M20" s="1">
-        <v>45.944336097651835</v>
-      </c>
-      <c r="N20" s="1">
-        <v>8.954968776351039E-16</v>
-      </c>
-      <c r="O20" s="1">
-        <v>0.3145494642941889</v>
-      </c>
-      <c r="P20" s="1">
-        <v>0.34559017820304588</v>
-      </c>
-      <c r="Q20" s="1">
-        <v>0.3145494642941889</v>
-      </c>
-      <c r="R20" s="1">
-        <v>0.34559017820304588</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B21" s="7">
+      <c r="D36">
+        <f>data!F36</f>
+        <v>30</v>
+      </c>
+      <c r="E36">
+        <f>data!I36</f>
+        <v>1.7</v>
+      </c>
+      <c r="F36">
+        <f>data!J36</f>
+        <v>3</v>
+      </c>
+      <c r="G36" s="7">
+        <f>regression!$L$18+regression!$L$19*B36+$L$20*C36+$L$21*D36+$L$22*E36+$L$23*F36</f>
+        <v>3.1488840550968904</v>
+      </c>
+      <c r="H36" s="9">
+        <f t="shared" si="0"/>
+        <v>3.4560011737028296</v>
+      </c>
+      <c r="I36" s="10">
+        <f t="shared" si="1"/>
+        <v>23.31003734379734</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="8">
+        <f>data!L37</f>
+        <v>32.35</v>
+      </c>
+      <c r="B37">
+        <f>data!B37</f>
         <v>12.5</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C37">
+        <f>data!C37</f>
         <v>2</v>
       </c>
-      <c r="D21" s="7">
-        <v>60</v>
-      </c>
-      <c r="E21" s="7">
-        <v>2.9750000000000001</v>
-      </c>
-      <c r="F21" s="7">
-        <v>3</v>
-      </c>
-      <c r="G21" s="8">
-        <f>regression!$K$18+regression!$K$19*B21+$K$20*C21+$K$21*D21+$K$22*E21+$K$23*F21</f>
-        <v>1.0154960799396342</v>
-      </c>
-      <c r="I21">
+      <c r="D37">
+        <f>data!F37</f>
+        <v>30</v>
+      </c>
+      <c r="E37">
+        <f>data!I37</f>
+        <v>1.7</v>
+      </c>
+      <c r="F37">
+        <f>data!J37</f>
+        <v>3</v>
+      </c>
+      <c r="G37" s="7">
+        <f>regression!$L$18+regression!$L$19*B37+$L$20*C37+$L$21*D37+$L$22*E37+$L$23*F37</f>
+        <v>3.1488840550968904</v>
+      </c>
+      <c r="H37" s="9">
+        <f t="shared" si="0"/>
+        <v>3.4766140209469096</v>
+      </c>
+      <c r="I37" s="10">
         <f t="shared" si="1"/>
-        <v>2.7607326017932237</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K21" s="1">
-        <v>-8.0542694847881069E-2</v>
-      </c>
-      <c r="L21" s="1">
-        <v>9.539826617491915E-4</v>
-      </c>
-      <c r="M21" s="1">
-        <v>-84.427839286094169</v>
-      </c>
-      <c r="N21" s="1">
-        <v>3.3739757992485499E-19</v>
-      </c>
-      <c r="O21" s="1">
-        <v>-8.2603649089132966E-2</v>
-      </c>
-      <c r="P21" s="1">
-        <v>-7.8481740606629172E-2</v>
-      </c>
-      <c r="Q21" s="1">
-        <v>-8.2603649089132966E-2</v>
-      </c>
-      <c r="R21" s="1">
-        <v>-7.8481740606629172E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B22" s="7">
-        <v>10</v>
-      </c>
-      <c r="C22" s="7">
-        <v>2</v>
-      </c>
-      <c r="D22" s="7">
-        <v>60</v>
-      </c>
-      <c r="E22" s="7">
-        <v>3</v>
-      </c>
-      <c r="F22" s="7">
-        <v>3</v>
-      </c>
-      <c r="G22" s="8">
-        <f>regression!$K$18+regression!$K$19*B22+$K$20*C22+$K$21*D22+$K$22*E22+$K$23*F22</f>
-        <v>1.1545375781965572</v>
-      </c>
-      <c r="I22">
-        <f t="shared" si="1"/>
-        <v>3.1725560191993365</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K22" s="1">
-        <v>0.29536762041227044</v>
-      </c>
-      <c r="L22" s="1">
-        <v>3.3336003860218573E-2</v>
-      </c>
-      <c r="M22" s="1">
-        <v>8.8603187607842386</v>
-      </c>
-      <c r="N22" s="1">
-        <v>7.1853157433204238E-7</v>
-      </c>
-      <c r="O22" s="1">
-        <v>0.22334956254093158</v>
-      </c>
-      <c r="P22" s="1">
-        <v>0.3673856782836093</v>
-      </c>
-      <c r="Q22" s="1">
-        <v>0.22334956254093158</v>
-      </c>
-      <c r="R22" s="1">
-        <v>0.3673856782836093</v>
-      </c>
-    </row>
-    <row r="23" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J23" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K23" s="2">
-        <v>0.75982235787432428</v>
-      </c>
-      <c r="L23" s="2">
-        <v>1.4232237863751135E-2</v>
-      </c>
-      <c r="M23" s="2">
-        <v>53.387412798204942</v>
-      </c>
-      <c r="N23" s="2">
-        <v>1.2839885751402051E-16</v>
-      </c>
-      <c r="O23" s="2">
-        <v>0.72907547728215338</v>
-      </c>
-      <c r="P23" s="2">
-        <v>0.79056923846649518</v>
-      </c>
-      <c r="Q23" s="2">
-        <v>0.72907547728215338</v>
-      </c>
-      <c r="R23" s="2">
-        <v>0.79056923846649518</v>
+        <v>23.31003734379734</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1">
-        <v>53.073031455920123</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>-2.8929084386167498</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>21.56150488413391</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4">
-        <v>-3.5392067626801311</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5">
-        <v>19.820227917869065</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>10.244112756484029</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updates to heat transfer model to report progress, specifiy starting date, albedo, and sky view factor in input parameters. updates to satellite validation to include processed output of ASTER images, other small updates.
</commit_message>
<xml_diff>
--- a/data/runtime-tracker.xlsx
+++ b/data/runtime-tracker.xlsx
@@ -2,18 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cghoehne\GitHub Projects\transport-uhi-phx\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\GitHub Projects\transport-uhi-phx\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8910" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8910"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
     <sheet name="regression" sheetId="5" r:id="rId2"/>
+    <sheet name="new-reg" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="solver_eng" localSheetId="1" hidden="1">1</definedName>
@@ -24,12 +25,12 @@
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>run.n</t>
   </si>
@@ -52,9 +53,6 @@
     <t>pave.length</t>
   </si>
   <si>
-    <t>layer.profile</t>
-  </si>
-  <si>
     <t>n.days</t>
   </si>
   <si>
@@ -65,9 +63,6 @@
   </si>
   <si>
     <t>CFL_fail</t>
-  </si>
-  <si>
-    <t>ref</t>
   </si>
   <si>
     <t>T.degC_Avg_Day_Max_0m</t>
@@ -104,9 +99,6 @@
   </si>
   <si>
     <t>depth</t>
-  </si>
-  <si>
-    <t>broke.t</t>
   </si>
   <si>
     <t>SUMMARY OUTPUT</t>
@@ -193,7 +185,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -724,7 +716,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -740,6 +732,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -799,7 +792,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1152,7 +1145,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0BBA-4AAB-B2C7-5CB90CCFF91D}"/>
             </c:ext>
@@ -1166,11 +1159,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="539167560"/>
-        <c:axId val="539164936"/>
+        <c:axId val="2102855280"/>
+        <c:axId val="2102858544"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="539167560"/>
+        <c:axId val="2102855280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1295,12 +1288,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539164936"/>
+        <c:crossAx val="2102858544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="539164936"/>
+        <c:axId val="2102858544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1425,7 +1418,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="539167560"/>
+        <c:crossAx val="2102855280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2323,15 +2316,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X37"/>
+  <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2354,16 +2347,16 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>24</v>
-      </c>
       <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
         <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>23</v>
       </c>
       <c r="L1" t="s">
         <v>9</v>
@@ -2375,37 +2368,28 @@
         <v>11</v>
       </c>
       <c r="O1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="P1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Q1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="R1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="S1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="T1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="U1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" t="s">
-        <v>19</v>
-      </c>
-      <c r="X1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2428,58 +2412,52 @@
         <v>10</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I2">
-        <v>2.2000000000000002</v>
+        <v>7</v>
       </c>
       <c r="J2">
-        <v>7</v>
+        <f>C2*I2*H2/F2/B2</f>
+        <v>0.20533333333333334</v>
       </c>
       <c r="K2">
-        <f>C2*J2*I2/F2/B2</f>
-        <v>0.20533333333333334</v>
+        <v>139.16999999999999</v>
       </c>
       <c r="L2">
-        <v>139.16999999999999</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
-      <c r="Q2" t="e">
-        <f t="shared" ref="Q2:R5" si="0">-Inf</f>
+        <v>1</v>
+      </c>
+      <c r="N2" t="e">
+        <f t="shared" ref="N2:O5" si="0">-Inf</f>
         <v>#NAME?</v>
       </c>
-      <c r="R2" t="e">
+      <c r="O2" t="e">
         <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
-      <c r="S2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T2">
+      <c r="P2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2">
         <v>5.1775850633579203</v>
       </c>
-      <c r="U2" t="s">
-        <v>21</v>
-      </c>
-      <c r="V2">
+      <c r="R2" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2">
         <v>5320302.5421906002</v>
       </c>
-      <c r="W2" t="s">
-        <v>21</v>
-      </c>
-      <c r="X2">
+      <c r="T2" t="s">
+        <v>19</v>
+      </c>
+      <c r="U2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2502,58 +2480,52 @@
         <v>75</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="I3">
-        <v>2.2000000000000002</v>
+        <v>7</v>
       </c>
       <c r="J3">
-        <v>7</v>
+        <f>C3*I3*H3/F3/B3</f>
+        <v>0.20533333333333334</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K37" si="1">C3*J3*I3/F3/B3</f>
-        <v>0.20533333333333334</v>
-      </c>
-      <c r="L3">
         <v>139.04</v>
       </c>
-      <c r="M3" t="s">
-        <v>22</v>
-      </c>
-      <c r="N3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
-      <c r="Q3" t="e">
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3" t="e">
         <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
-      <c r="R3" t="e">
+      <c r="O3" t="e">
         <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
-      <c r="S3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T3">
+      <c r="P3" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q3">
         <v>4.7402378917359398</v>
       </c>
-      <c r="U3" t="s">
-        <v>21</v>
-      </c>
-      <c r="V3">
+      <c r="R3" t="s">
+        <v>19</v>
+      </c>
+      <c r="S3">
         <v>4848514.72147673</v>
       </c>
-      <c r="W3" t="s">
-        <v>21</v>
-      </c>
-      <c r="X3">
+      <c r="T3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2576,58 +2548,52 @@
         <v>10</v>
       </c>
       <c r="H4">
-        <v>2</v>
+        <v>2.1749999999999998</v>
       </c>
       <c r="I4">
-        <v>2.1749999999999998</v>
+        <v>7</v>
       </c>
       <c r="J4">
-        <v>7</v>
+        <f>C4*I4*H4/F4/B4</f>
+        <v>0.20300000000000001</v>
       </c>
       <c r="K4">
-        <f t="shared" si="1"/>
-        <v>0.20300000000000001</v>
+        <v>137.76</v>
       </c>
       <c r="L4">
-        <v>137.76</v>
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>0</v>
-      </c>
-      <c r="N4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>3</v>
-      </c>
-      <c r="Q4" t="e">
+        <v>1</v>
+      </c>
+      <c r="N4" t="e">
         <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
-      <c r="R4" t="e">
+      <c r="O4" t="e">
         <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
-      <c r="S4" t="s">
-        <v>21</v>
-      </c>
-      <c r="T4">
+      <c r="P4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q4">
         <v>1162.7146996675799</v>
       </c>
-      <c r="U4" t="s">
-        <v>21</v>
-      </c>
-      <c r="V4">
+      <c r="R4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S4">
         <v>14.9468298314299</v>
       </c>
-      <c r="W4" t="s">
-        <v>21</v>
-      </c>
-      <c r="X4">
+      <c r="T4" t="s">
+        <v>19</v>
+      </c>
+      <c r="U4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2650,58 +2616,52 @@
         <v>75</v>
       </c>
       <c r="H5">
-        <v>2</v>
+        <v>2.1749999999999998</v>
       </c>
       <c r="I5">
-        <v>2.1749999999999998</v>
+        <v>7</v>
       </c>
       <c r="J5">
-        <v>7</v>
+        <f>C5*I5*H5/F5/B5</f>
+        <v>0.20300000000000001</v>
       </c>
       <c r="K5">
-        <f t="shared" si="1"/>
-        <v>0.20300000000000001</v>
-      </c>
-      <c r="L5">
         <v>138.04</v>
       </c>
-      <c r="M5" t="s">
-        <v>22</v>
-      </c>
-      <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>3</v>
-      </c>
-      <c r="Q5" t="e">
+      <c r="L5" t="s">
+        <v>20</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5" t="e">
         <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
-      <c r="R5" t="e">
+      <c r="O5" t="e">
         <f t="shared" si="0"/>
         <v>#NAME?</v>
       </c>
-      <c r="S5" t="s">
-        <v>21</v>
-      </c>
-      <c r="T5">
+      <c r="P5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q5">
         <v>1034.28594240245</v>
       </c>
-      <c r="U5" t="s">
-        <v>21</v>
-      </c>
-      <c r="V5">
+      <c r="R5" t="s">
+        <v>19</v>
+      </c>
+      <c r="S5">
         <v>15.8599314157618</v>
       </c>
-      <c r="W5" t="s">
-        <v>21</v>
-      </c>
-      <c r="X5">
+      <c r="T5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2724,59 +2684,50 @@
         <v>10</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>2.8</v>
       </c>
       <c r="I6">
-        <v>2.8</v>
+        <v>1</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <f>C6*I6*H6/F6/B6</f>
+        <v>9.3333333333333324E-3</v>
       </c>
       <c r="K6">
-        <f t="shared" si="1"/>
-        <v>9.3333333333333324E-3</v>
-      </c>
-      <c r="L6">
         <v>5.27</v>
       </c>
-      <c r="M6" t="s">
-        <v>21</v>
+      <c r="L6" t="s">
+        <v>19</v>
+      </c>
+      <c r="M6">
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6" t="s">
-        <v>22</v>
+        <v>68.957038853210094</v>
+      </c>
+      <c r="O6">
+        <v>73.106567382231603</v>
       </c>
       <c r="P6">
-        <v>1</v>
+        <v>44.235637155873199</v>
       </c>
       <c r="Q6">
-        <v>68.957038853210094</v>
+        <v>23.401076055063999</v>
       </c>
       <c r="R6">
-        <v>73.106567382231603</v>
+        <v>26.866506382396899</v>
       </c>
       <c r="S6">
-        <v>44.235637155873199</v>
+        <v>12.845554393268699</v>
       </c>
       <c r="T6">
-        <v>23.401076055063999</v>
+        <v>17.434943750180398</v>
       </c>
       <c r="U6">
-        <v>26.866506382396899</v>
-      </c>
-      <c r="V6">
-        <v>12.845554393268699</v>
-      </c>
-      <c r="W6">
-        <v>17.434943750180398</v>
-      </c>
-      <c r="X6">
         <v>1.1234305929974701E-8</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2799,59 +2750,50 @@
         <v>10</v>
       </c>
       <c r="H7">
-        <v>1</v>
+        <v>2.8</v>
       </c>
       <c r="I7">
-        <v>2.8</v>
+        <v>1</v>
       </c>
       <c r="J7">
-        <v>1</v>
+        <f>C7*I7*H7/F7/B7</f>
+        <v>7.4666666666666657E-3</v>
       </c>
       <c r="K7">
-        <f t="shared" si="1"/>
-        <v>7.4666666666666657E-3</v>
-      </c>
-      <c r="L7">
         <v>4.05</v>
       </c>
-      <c r="M7" t="s">
-        <v>21</v>
+      <c r="L7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7" t="s">
-        <v>22</v>
+        <v>69.155007905735403</v>
+      </c>
+      <c r="O7">
+        <v>73.287134611134505</v>
       </c>
       <c r="P7">
-        <v>1</v>
+        <v>43.804607497918497</v>
       </c>
       <c r="Q7">
-        <v>69.155007905735403</v>
+        <v>23.611228907385499</v>
       </c>
       <c r="R7">
-        <v>73.287134611134505</v>
+        <v>26.855414215114902</v>
       </c>
       <c r="S7">
-        <v>43.804607497918497</v>
+        <v>13.116753731338999</v>
       </c>
       <c r="T7">
-        <v>23.611228907385499</v>
+        <v>17.444190295325701</v>
       </c>
       <c r="U7">
-        <v>26.855414215114902</v>
-      </c>
-      <c r="V7">
-        <v>13.116753731338999</v>
-      </c>
-      <c r="W7">
-        <v>17.444190295325701</v>
-      </c>
-      <c r="X7">
         <v>9.1868059826083498E-9</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -2874,59 +2816,50 @@
         <v>10</v>
       </c>
       <c r="H8">
-        <v>1</v>
+        <v>2.8</v>
       </c>
       <c r="I8">
-        <v>2.8</v>
+        <v>1</v>
       </c>
       <c r="J8">
-        <v>1</v>
+        <f>C8*I8*H8/F8/B8</f>
+        <v>4.6666666666666662E-3</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
-        <v>4.6666666666666662E-3</v>
-      </c>
-      <c r="L8">
         <v>1.7</v>
       </c>
-      <c r="M8" t="s">
-        <v>21</v>
+      <c r="L8" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
       </c>
       <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8" t="s">
-        <v>22</v>
+        <v>68.777015902481594</v>
+      </c>
+      <c r="O8">
+        <v>72.936197871854205</v>
       </c>
       <c r="P8">
-        <v>1</v>
+        <v>44.043276681267301</v>
       </c>
       <c r="Q8">
-        <v>68.777015902481594</v>
+        <v>23.195690651191001</v>
       </c>
       <c r="R8">
-        <v>72.936197871854205</v>
+        <v>26.556193522340699</v>
       </c>
       <c r="S8">
-        <v>44.043276681267301</v>
+        <v>12.655777116750899</v>
       </c>
       <c r="T8">
-        <v>23.195690651191001</v>
+        <v>17.218530373050299</v>
       </c>
       <c r="U8">
-        <v>26.556193522340699</v>
-      </c>
-      <c r="V8">
-        <v>12.655777116750899</v>
-      </c>
-      <c r="W8">
-        <v>17.218530373050299</v>
-      </c>
-      <c r="X8">
         <v>1.13843441340578E-8</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -2949,59 +2882,50 @@
         <v>10</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>2.8</v>
       </c>
       <c r="I9">
-        <v>2.8</v>
+        <v>1</v>
       </c>
       <c r="J9">
-        <v>1</v>
+        <f>C9*I9*H9/F9/B9</f>
+        <v>3.7333333333333329E-3</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
-        <v>3.7333333333333329E-3</v>
-      </c>
-      <c r="L9">
         <v>1.52</v>
       </c>
-      <c r="M9" t="s">
-        <v>21</v>
+      <c r="L9" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
       </c>
       <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9" t="s">
-        <v>22</v>
+        <v>69.001868703716099</v>
+      </c>
+      <c r="O9">
+        <v>73.139813147918602</v>
       </c>
       <c r="P9">
-        <v>1</v>
+        <v>43.650946687239298</v>
       </c>
       <c r="Q9">
-        <v>69.001868703716099</v>
+        <v>23.477857422986801</v>
       </c>
       <c r="R9">
-        <v>73.139813147918602</v>
+        <v>26.612189512259899</v>
       </c>
       <c r="S9">
-        <v>43.650946687239298</v>
+        <v>12.952613931387701</v>
       </c>
       <c r="T9">
-        <v>23.477857422986801</v>
+        <v>17.281439807510498</v>
       </c>
       <c r="U9">
-        <v>26.612189512259899</v>
-      </c>
-      <c r="V9">
-        <v>12.952613931387701</v>
-      </c>
-      <c r="W9">
-        <v>17.281439807510498</v>
-      </c>
-      <c r="X9">
         <v>1.00064880825812E-8</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3024,59 +2948,50 @@
         <v>10</v>
       </c>
       <c r="H10">
-        <v>1</v>
+        <v>2.8</v>
       </c>
       <c r="I10">
-        <v>2.8</v>
+        <v>1</v>
       </c>
       <c r="J10">
-        <v>1</v>
+        <f>C10*I10*H10/F10/B10</f>
+        <v>1.8666666666666664E-3</v>
       </c>
       <c r="K10">
-        <f t="shared" si="1"/>
-        <v>1.8666666666666664E-3</v>
-      </c>
-      <c r="L10">
         <v>0.75</v>
       </c>
-      <c r="M10" t="s">
-        <v>21</v>
+      <c r="L10" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
       </c>
       <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10" t="s">
-        <v>22</v>
+        <v>68.540190444836995</v>
+      </c>
+      <c r="O10">
+        <v>72.673040331112603</v>
       </c>
       <c r="P10">
-        <v>1</v>
+        <v>43.713698849225899</v>
       </c>
       <c r="Q10">
-        <v>68.540190444836995</v>
+        <v>24.051239563063699</v>
       </c>
       <c r="R10">
-        <v>72.673040331112603</v>
+        <v>26.457493121210501</v>
       </c>
       <c r="S10">
-        <v>43.713698849225899</v>
+        <v>12.979451773627</v>
       </c>
       <c r="T10">
-        <v>24.051239563063699</v>
+        <v>17.300033996161499</v>
       </c>
       <c r="U10">
-        <v>26.457493121210501</v>
-      </c>
-      <c r="V10">
-        <v>12.979451773627</v>
-      </c>
-      <c r="W10">
-        <v>17.300033996161499</v>
-      </c>
-      <c r="X10">
         <v>3.1693625146544898E-7</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>11</v>
       </c>
@@ -3099,59 +3014,50 @@
         <v>10</v>
       </c>
       <c r="H11">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="I11">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <f>C11*I11*H11/F11/B11</f>
+        <v>1.6666666666666666E-3</v>
       </c>
       <c r="K11">
-        <f t="shared" si="1"/>
-        <v>1.6666666666666666E-3</v>
+        <v>2.52</v>
       </c>
       <c r="L11">
-        <v>2.52</v>
+        <v>6.0770880308972899</v>
       </c>
       <c r="M11">
-        <v>6.0770880308972899</v>
+        <v>0</v>
       </c>
       <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11" t="s">
-        <v>22</v>
+        <v>71.698043059591797</v>
+      </c>
+      <c r="O11">
+        <v>77.7719230425365</v>
       </c>
       <c r="P11">
-        <v>10</v>
+        <v>49.223957657734601</v>
       </c>
       <c r="Q11">
-        <v>71.698043059591797</v>
+        <v>22.702600328705302</v>
       </c>
       <c r="R11">
-        <v>77.7719230425365</v>
+        <v>26.6869783459011</v>
       </c>
       <c r="S11">
-        <v>49.223957657734601</v>
+        <v>14.815435031141799</v>
       </c>
       <c r="T11">
-        <v>22.702600328705302</v>
+        <v>21.703233280833</v>
       </c>
       <c r="U11">
-        <v>26.6869783459011</v>
-      </c>
-      <c r="V11">
-        <v>14.815435031141799</v>
-      </c>
-      <c r="W11">
-        <v>21.703233280833</v>
-      </c>
-      <c r="X11">
         <v>1.68867171706211E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>12</v>
       </c>
@@ -3174,59 +3080,50 @@
         <v>10</v>
       </c>
       <c r="H12">
-        <v>2</v>
+        <v>0.5</v>
       </c>
       <c r="I12">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <f>C12*I12*H12/F12/B12</f>
+        <v>1.3333333333333333E-3</v>
       </c>
       <c r="K12">
-        <f t="shared" si="1"/>
-        <v>1.3333333333333333E-3</v>
+        <v>2.44</v>
       </c>
       <c r="L12">
-        <v>2.44</v>
+        <v>6.9703339564717401E+126</v>
       </c>
       <c r="M12">
-        <v>6.9703339564717401E+126</v>
+        <v>0</v>
       </c>
       <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12" t="s">
-        <v>22</v>
+        <v>71.874794786634993</v>
+      </c>
+      <c r="O12">
+        <v>77.905789321712902</v>
       </c>
       <c r="P12">
-        <v>10</v>
+        <v>48.612661676941997</v>
       </c>
       <c r="Q12">
-        <v>71.874794786634993</v>
+        <v>23.279567009550998</v>
       </c>
       <c r="R12">
-        <v>77.905789321712902</v>
+        <v>27.055662332744198</v>
       </c>
       <c r="S12">
-        <v>48.612661676941997</v>
+        <v>15.1737378568608</v>
       </c>
       <c r="T12">
-        <v>23.279567009550998</v>
+        <v>21.6671031922005</v>
       </c>
       <c r="U12">
-        <v>27.055662332744198</v>
-      </c>
-      <c r="V12">
-        <v>15.1737378568608</v>
-      </c>
-      <c r="W12">
-        <v>21.6671031922005</v>
-      </c>
-      <c r="X12">
         <v>1.7812546544092801E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>20</v>
       </c>
@@ -3249,59 +3146,50 @@
         <v>10</v>
       </c>
       <c r="H13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J13">
-        <v>1</v>
+        <f>C13*I13*H13/F13/B13</f>
+        <v>6.6666666666666662E-3</v>
       </c>
       <c r="K13">
-        <f t="shared" si="1"/>
-        <v>6.6666666666666662E-3</v>
+        <v>3.69</v>
       </c>
       <c r="L13">
-        <v>3.69</v>
+        <v>8.6577218581061504E+17</v>
       </c>
       <c r="M13">
-        <v>8.6577218581061504E+17</v>
+        <v>0</v>
       </c>
       <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13" t="s">
-        <v>22</v>
+        <v>72.082818613926094</v>
+      </c>
+      <c r="O13">
+        <v>73.810833389213798</v>
       </c>
       <c r="P13">
-        <v>19</v>
+        <v>46.558785235214501</v>
       </c>
       <c r="Q13">
-        <v>72.082818613926094</v>
+        <v>31.6710364749914</v>
       </c>
       <c r="R13">
-        <v>73.810833389213798</v>
+        <v>40.819112958815502</v>
       </c>
       <c r="S13">
-        <v>46.558785235214501</v>
+        <v>24.657545014066599</v>
       </c>
       <c r="T13">
-        <v>31.6710364749914</v>
+        <v>29.1207948176855</v>
       </c>
       <c r="U13">
-        <v>40.819112958815502</v>
-      </c>
-      <c r="V13">
-        <v>24.657545014066599</v>
-      </c>
-      <c r="W13">
-        <v>29.1207948176855</v>
-      </c>
-      <c r="X13">
         <v>6.28459901008682E-7</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>21</v>
       </c>
@@ -3324,59 +3212,50 @@
         <v>10</v>
       </c>
       <c r="H14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I14">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J14">
-        <v>1</v>
+        <f>C14*I14*H14/F14/B14</f>
+        <v>5.3333333333333332E-3</v>
       </c>
       <c r="K14">
-        <f t="shared" si="1"/>
-        <v>5.3333333333333332E-3</v>
+        <v>3.34</v>
       </c>
       <c r="L14">
-        <v>3.34</v>
+        <v>3.9042917094357699</v>
       </c>
       <c r="M14">
-        <v>3.9042917094357699</v>
+        <v>0</v>
       </c>
       <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14" t="s">
-        <v>22</v>
+        <v>67.798581802435095</v>
+      </c>
+      <c r="O14">
+        <v>69.965053450135997</v>
       </c>
       <c r="P14">
-        <v>19</v>
+        <v>41.216565691395203</v>
       </c>
       <c r="Q14">
-        <v>67.798581802435095</v>
+        <v>27.264787033129402</v>
       </c>
       <c r="R14">
-        <v>69.965053450135997</v>
+        <v>33.868724128293103</v>
       </c>
       <c r="S14">
-        <v>41.216565691395203</v>
+        <v>20.4225516399983</v>
       </c>
       <c r="T14">
-        <v>27.264787033129402</v>
+        <v>24.2079692174675</v>
       </c>
       <c r="U14">
-        <v>33.868724128293103</v>
-      </c>
-      <c r="V14">
-        <v>20.4225516399983</v>
-      </c>
-      <c r="W14">
-        <v>24.2079692174675</v>
-      </c>
-      <c r="X14">
         <v>6.0370766163941901E-7</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>24</v>
       </c>
@@ -3399,59 +3278,50 @@
         <v>10</v>
       </c>
       <c r="H15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J15">
-        <v>1</v>
+        <f>C15*I15*H15/F15/B15</f>
+        <v>2.6666666666666666E-3</v>
       </c>
       <c r="K15">
-        <f t="shared" si="1"/>
-        <v>2.6666666666666666E-3</v>
+        <v>1.36</v>
       </c>
       <c r="L15">
-        <v>1.36</v>
+        <v>3.85153464796824</v>
       </c>
       <c r="M15">
-        <v>3.85153464796824</v>
+        <v>0</v>
       </c>
       <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15" t="s">
-        <v>22</v>
+        <v>67.384388585429306</v>
+      </c>
+      <c r="O15">
+        <v>69.522995278094399</v>
       </c>
       <c r="P15">
-        <v>19</v>
+        <v>40.747585322674702</v>
       </c>
       <c r="Q15">
-        <v>67.384388585429306</v>
+        <v>26.986544430155799</v>
       </c>
       <c r="R15">
-        <v>69.522995278094399</v>
+        <v>33.357451708997701</v>
       </c>
       <c r="S15">
-        <v>40.747585322674702</v>
+        <v>20.124221914940101</v>
       </c>
       <c r="T15">
-        <v>26.986544430155799</v>
+        <v>23.818372565913801</v>
       </c>
       <c r="U15">
-        <v>33.357451708997701</v>
-      </c>
-      <c r="V15">
-        <v>20.124221914940101</v>
-      </c>
-      <c r="W15">
-        <v>23.818372565913801</v>
-      </c>
-      <c r="X15">
         <v>7.3980950787699797E-7</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>
@@ -3474,59 +3344,50 @@
         <v>10</v>
       </c>
       <c r="H16">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I16">
         <v>3</v>
       </c>
       <c r="J16">
-        <v>3</v>
+        <f>C16*I16*H16/F16/B16</f>
+        <v>0.06</v>
       </c>
       <c r="K16">
-        <f t="shared" si="1"/>
-        <v>0.06</v>
+        <v>88.24</v>
       </c>
       <c r="L16">
-        <v>88.24</v>
+        <v>0</v>
       </c>
       <c r="M16">
         <v>0</v>
       </c>
       <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16" t="s">
-        <v>22</v>
+        <v>74.362483112893401</v>
+      </c>
+      <c r="O16">
+        <v>78.491203611156706</v>
       </c>
       <c r="P16">
-        <v>1</v>
+        <v>49.819399412175201</v>
       </c>
       <c r="Q16">
-        <v>74.362483112893401</v>
+        <v>20.4598094402788</v>
       </c>
       <c r="R16">
-        <v>78.491203611156706</v>
+        <v>32.938328313601197</v>
       </c>
       <c r="S16">
-        <v>49.819399412175201</v>
+        <v>10.5107147598357</v>
       </c>
       <c r="T16">
-        <v>20.4598094402788</v>
+        <v>23.578515749764801</v>
       </c>
       <c r="U16">
-        <v>32.938328313601197</v>
-      </c>
-      <c r="V16">
-        <v>10.5107147598357</v>
-      </c>
-      <c r="W16">
-        <v>23.578515749764801</v>
-      </c>
-      <c r="X16">
         <v>3.1085913825563698E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2</v>
       </c>
@@ -3549,59 +3410,50 @@
         <v>10</v>
       </c>
       <c r="H17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I17">
         <v>3</v>
       </c>
       <c r="J17">
-        <v>3</v>
+        <f>C17*I17*H17/F17/B17</f>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="K17">
-        <f t="shared" si="1"/>
-        <v>4.8000000000000001E-2</v>
+        <v>72.930000000000007</v>
       </c>
       <c r="L17">
-        <v>72.930000000000007</v>
+        <v>3.8058879799663999E-2</v>
       </c>
       <c r="M17">
-        <v>3.8058879799663999E-2</v>
+        <v>0</v>
       </c>
       <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17" t="s">
-        <v>22</v>
+        <v>74.507439778758297</v>
+      </c>
+      <c r="O17">
+        <v>78.620423294330493</v>
       </c>
       <c r="P17">
-        <v>1</v>
+        <v>49.377975146098002</v>
       </c>
       <c r="Q17">
-        <v>74.507439778758297</v>
+        <v>20.773907954103102</v>
       </c>
       <c r="R17">
-        <v>78.620423294330493</v>
+        <v>32.8661404536455</v>
       </c>
       <c r="S17">
-        <v>49.377975146098002</v>
+        <v>10.694441375236201</v>
       </c>
       <c r="T17">
-        <v>20.773907954103102</v>
+        <v>23.536202667985599</v>
       </c>
       <c r="U17">
-        <v>32.8661404536455</v>
-      </c>
-      <c r="V17">
-        <v>10.694441375236201</v>
-      </c>
-      <c r="W17">
-        <v>23.536202667985599</v>
-      </c>
-      <c r="X17">
         <v>3.3708501611329198E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>3</v>
       </c>
@@ -3624,59 +3476,50 @@
         <v>10</v>
       </c>
       <c r="H18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I18">
         <v>3</v>
       </c>
       <c r="J18">
-        <v>3</v>
+        <f>C18*I18*H18/F18/B18</f>
+        <v>0.04</v>
       </c>
       <c r="K18">
-        <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>65.73</v>
       </c>
       <c r="L18">
-        <v>65.73</v>
+        <v>0.71645347708618901</v>
       </c>
       <c r="M18">
-        <v>0.71645347708618901</v>
+        <v>0</v>
       </c>
       <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18" t="s">
-        <v>22</v>
+        <v>76.486791848695901</v>
+      </c>
+      <c r="O18">
+        <v>80.679801587052907</v>
       </c>
       <c r="P18">
-        <v>1</v>
+        <v>51.513169628137099</v>
       </c>
       <c r="Q18">
-        <v>76.486791848695901</v>
+        <v>22.210120520090999</v>
       </c>
       <c r="R18">
-        <v>80.679801587052907</v>
+        <v>38.248507108265301</v>
       </c>
       <c r="S18">
-        <v>51.513169628137099</v>
+        <v>13.4025883387707</v>
       </c>
       <c r="T18">
-        <v>22.210120520090999</v>
+        <v>28.859195798987901</v>
       </c>
       <c r="U18">
-        <v>38.248507108265301</v>
-      </c>
-      <c r="V18">
-        <v>13.4025883387707</v>
-      </c>
-      <c r="W18">
-        <v>28.859195798987901</v>
-      </c>
-      <c r="X18">
         <v>4.2517938278336899E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>4</v>
       </c>
@@ -3699,59 +3542,50 @@
         <v>10</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I19">
         <v>3</v>
       </c>
       <c r="J19">
-        <v>3</v>
+        <f>C19*I19*H19/F19/B19</f>
+        <v>0.03</v>
       </c>
       <c r="K19">
-        <f t="shared" si="1"/>
-        <v>0.03</v>
+        <v>24.57</v>
       </c>
       <c r="L19">
-        <v>24.57</v>
+        <v>1.95216818864083E-2</v>
       </c>
       <c r="M19">
-        <v>1.95216818864083E-2</v>
+        <v>0</v>
       </c>
       <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19" t="s">
-        <v>22</v>
+        <v>74.283234023094494</v>
+      </c>
+      <c r="O19">
+        <v>78.418450397283806</v>
       </c>
       <c r="P19">
-        <v>1</v>
+        <v>49.7531086510851</v>
       </c>
       <c r="Q19">
-        <v>74.283234023094494</v>
+        <v>20.337120403767099</v>
       </c>
       <c r="R19">
-        <v>78.418450397283806</v>
+        <v>32.819077237964301</v>
       </c>
       <c r="S19">
-        <v>49.7531086510851</v>
+        <v>10.4419337361186</v>
       </c>
       <c r="T19">
-        <v>20.337120403767099</v>
+        <v>23.4972792142784</v>
       </c>
       <c r="U19">
-        <v>32.819077237964301</v>
-      </c>
-      <c r="V19">
-        <v>10.4419337361186</v>
-      </c>
-      <c r="W19">
-        <v>23.4972792142784</v>
-      </c>
-      <c r="X19">
         <v>2.9248499121194999E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>5</v>
       </c>
@@ -3774,59 +3608,50 @@
         <v>10</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I20">
         <v>3</v>
       </c>
       <c r="J20">
-        <v>3</v>
+        <f>C20*I20*H20/F20/B20</f>
+        <v>2.4E-2</v>
       </c>
       <c r="K20">
-        <f t="shared" si="1"/>
-        <v>2.4E-2</v>
+        <v>22.46</v>
       </c>
       <c r="L20">
-        <v>22.46</v>
+        <v>2.0513240908944699E-2</v>
       </c>
       <c r="M20">
-        <v>2.0513240908944699E-2</v>
+        <v>0</v>
       </c>
       <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20" t="s">
-        <v>22</v>
+        <v>74.443400174725696</v>
+      </c>
+      <c r="O20">
+        <v>78.560655345219601</v>
       </c>
       <c r="P20">
-        <v>1</v>
+        <v>49.311567846658697</v>
       </c>
       <c r="Q20">
-        <v>74.443400174725696</v>
+        <v>20.662573316873399</v>
       </c>
       <c r="R20">
-        <v>78.560655345219601</v>
+        <v>32.759681279735702</v>
       </c>
       <c r="S20">
-        <v>49.311567846658697</v>
+        <v>10.6142384296255</v>
       </c>
       <c r="T20">
-        <v>20.662573316873399</v>
+        <v>23.462409324805702</v>
       </c>
       <c r="U20">
-        <v>32.759681279735702</v>
-      </c>
-      <c r="V20">
-        <v>10.6142384296255</v>
-      </c>
-      <c r="W20">
-        <v>23.462409324805702</v>
-      </c>
-      <c r="X20">
         <v>3.2405109165267701E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6</v>
       </c>
@@ -3849,59 +3674,50 @@
         <v>10</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I21">
         <v>3</v>
       </c>
       <c r="J21">
-        <v>3</v>
+        <f>C21*I21*H21/F21/B21</f>
+        <v>0.02</v>
       </c>
       <c r="K21">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
+        <v>20.260000000000002</v>
       </c>
       <c r="L21">
-        <v>20.260000000000002</v>
+        <v>0.70733782141243895</v>
       </c>
       <c r="M21">
-        <v>0.70733782141243895</v>
+        <v>0</v>
       </c>
       <c r="N21">
-        <v>0</v>
-      </c>
-      <c r="O21" t="s">
-        <v>22</v>
+        <v>76.426448411096203</v>
+      </c>
+      <c r="O21">
+        <v>80.628479456753396</v>
       </c>
       <c r="P21">
-        <v>1</v>
+        <v>51.461249286803998</v>
       </c>
       <c r="Q21">
-        <v>76.426448411096203</v>
+        <v>22.092311175135301</v>
       </c>
       <c r="R21">
-        <v>80.628479456753396</v>
+        <v>38.153108294861198</v>
       </c>
       <c r="S21">
-        <v>51.461249286803998</v>
+        <v>13.3384634655954</v>
       </c>
       <c r="T21">
-        <v>22.092311175135301</v>
+        <v>28.790314587491899</v>
       </c>
       <c r="U21">
-        <v>38.153108294861198</v>
-      </c>
-      <c r="V21">
-        <v>13.3384634655954</v>
-      </c>
-      <c r="W21">
-        <v>28.790314587491899</v>
-      </c>
-      <c r="X21">
         <v>4.0824982139042697E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>7</v>
       </c>
@@ -3924,59 +3740,50 @@
         <v>10</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I22">
         <v>3</v>
       </c>
       <c r="J22">
-        <v>3</v>
+        <f>C22*I22*H22/F22/B22</f>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="K22">
-        <f t="shared" si="1"/>
-        <v>1.4999999999999999E-2</v>
+        <v>8.2899999999999991</v>
       </c>
       <c r="L22">
-        <v>8.2899999999999991</v>
+        <v>5.7002718371641399E-2</v>
       </c>
       <c r="M22">
-        <v>5.7002718371641399E-2</v>
+        <v>0</v>
       </c>
       <c r="N22">
-        <v>0</v>
-      </c>
-      <c r="O22" t="s">
-        <v>22</v>
+        <v>74.133183352360703</v>
+      </c>
+      <c r="O22">
+        <v>78.278944706861395</v>
       </c>
       <c r="P22">
-        <v>1</v>
+        <v>49.598203000512903</v>
       </c>
       <c r="Q22">
-        <v>74.133183352360703</v>
+        <v>20.100944665816101</v>
       </c>
       <c r="R22">
-        <v>78.278944706861395</v>
+        <v>32.559295705121698</v>
       </c>
       <c r="S22">
-        <v>49.598203000512903</v>
+        <v>10.2981459911082</v>
       </c>
       <c r="T22">
-        <v>20.100944665816101</v>
+        <v>23.311814820034201</v>
       </c>
       <c r="U22">
-        <v>32.559295705121698</v>
-      </c>
-      <c r="V22">
-        <v>10.2981459911082</v>
-      </c>
-      <c r="W22">
-        <v>23.311814820034201</v>
-      </c>
-      <c r="X22">
         <v>2.6585238135794502E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>8</v>
       </c>
@@ -3999,59 +3806,50 @@
         <v>10</v>
       </c>
       <c r="H23">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I23">
         <v>3</v>
       </c>
       <c r="J23">
-        <v>3</v>
+        <f>C23*I23*H23/F23/B23</f>
+        <v>1.2E-2</v>
       </c>
       <c r="K23">
-        <f t="shared" si="1"/>
-        <v>1.2E-2</v>
+        <v>7.37</v>
       </c>
       <c r="L23">
-        <v>7.37</v>
+        <v>1.5524390332856399E-2</v>
       </c>
       <c r="M23">
-        <v>1.5524390332856399E-2</v>
+        <v>0</v>
       </c>
       <c r="N23">
-        <v>0</v>
-      </c>
-      <c r="O23" t="s">
-        <v>22</v>
+        <v>74.317092657838501</v>
+      </c>
+      <c r="O23">
+        <v>78.444128627112093</v>
       </c>
       <c r="P23">
-        <v>1</v>
+        <v>49.1954515524668</v>
       </c>
       <c r="Q23">
-        <v>74.317092657838501</v>
+        <v>20.4382944389077</v>
       </c>
       <c r="R23">
-        <v>78.444128627112093</v>
+        <v>32.563259912113502</v>
       </c>
       <c r="S23">
-        <v>49.1954515524668</v>
+        <v>10.482705229971099</v>
       </c>
       <c r="T23">
-        <v>20.4382944389077</v>
+        <v>23.329418181358001</v>
       </c>
       <c r="U23">
-        <v>32.563259912113502</v>
-      </c>
-      <c r="V23">
-        <v>10.482705229971099</v>
-      </c>
-      <c r="W23">
-        <v>23.329418181358001</v>
-      </c>
-      <c r="X23">
         <v>2.95741080054768E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>9</v>
       </c>
@@ -4074,59 +3872,50 @@
         <v>10</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I24">
         <v>3</v>
       </c>
       <c r="J24">
-        <v>3</v>
+        <f>C24*I24*H24/F24/B24</f>
+        <v>0.01</v>
       </c>
       <c r="K24">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
+        <v>6.87</v>
       </c>
       <c r="L24">
-        <v>6.87</v>
+        <v>0.698130957754169</v>
       </c>
       <c r="M24">
-        <v>0.698130957754169</v>
+        <v>0</v>
       </c>
       <c r="N24">
-        <v>0</v>
-      </c>
-      <c r="O24" t="s">
-        <v>22</v>
+        <v>76.296594773239406</v>
+      </c>
+      <c r="O24">
+        <v>80.525119515017394</v>
       </c>
       <c r="P24">
-        <v>1</v>
+        <v>51.453844301385097</v>
       </c>
       <c r="Q24">
-        <v>76.296594773239406</v>
+        <v>21.896643756807102</v>
       </c>
       <c r="R24">
-        <v>80.525119515017394</v>
+        <v>38.056717766502203</v>
       </c>
       <c r="S24">
-        <v>51.453844301385097</v>
+        <v>13.229357160621401</v>
       </c>
       <c r="T24">
-        <v>21.896643756807102</v>
+        <v>28.743542103661099</v>
       </c>
       <c r="U24">
-        <v>38.056717766502203</v>
-      </c>
-      <c r="V24">
-        <v>13.229357160621401</v>
-      </c>
-      <c r="W24">
-        <v>28.743542103661099</v>
-      </c>
-      <c r="X24">
         <v>3.4716152103015899E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>10</v>
       </c>
@@ -4149,59 +3938,50 @@
         <v>50</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I25">
         <v>3</v>
       </c>
       <c r="J25">
-        <v>3</v>
+        <f>C25*I25*H25/F25/B25</f>
+        <v>0.06</v>
       </c>
       <c r="K25">
-        <f t="shared" si="1"/>
-        <v>0.06</v>
+        <v>88.38</v>
       </c>
       <c r="L25">
-        <v>88.38</v>
+        <v>0.24695675068206099</v>
       </c>
       <c r="M25">
-        <v>0.24695675068206099</v>
+        <v>0</v>
       </c>
       <c r="N25">
-        <v>0</v>
-      </c>
-      <c r="O25" t="s">
-        <v>22</v>
+        <v>77.934909175448794</v>
+      </c>
+      <c r="O25">
+        <v>82.168256335699994</v>
       </c>
       <c r="P25">
-        <v>1</v>
+        <v>53.291410376960201</v>
       </c>
       <c r="Q25">
-        <v>77.934909175448794</v>
+        <v>21.393785098721999</v>
       </c>
       <c r="R25">
-        <v>82.168256335699994</v>
+        <v>35.3928098851339</v>
       </c>
       <c r="S25">
-        <v>53.291410376960201</v>
+        <v>11.2338796265753</v>
       </c>
       <c r="T25">
-        <v>21.393785098721999</v>
+        <v>25.341865786308599</v>
       </c>
       <c r="U25">
-        <v>35.3928098851339</v>
-      </c>
-      <c r="V25">
-        <v>11.2338796265753</v>
-      </c>
-      <c r="W25">
-        <v>25.341865786308599</v>
-      </c>
-      <c r="X25">
         <v>3.7206910852489701E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>11</v>
       </c>
@@ -4224,59 +4004,50 @@
         <v>50</v>
       </c>
       <c r="H26">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I26">
         <v>3</v>
       </c>
       <c r="J26">
-        <v>3</v>
+        <f>C26*I26*H26/F26/B26</f>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="K26">
-        <f t="shared" si="1"/>
-        <v>4.8000000000000001E-2</v>
+        <v>73.42</v>
       </c>
       <c r="L26">
-        <v>73.42</v>
+        <v>0.29812611805786898</v>
       </c>
       <c r="M26">
-        <v>0.29812611805786898</v>
+        <v>0</v>
       </c>
       <c r="N26">
-        <v>0</v>
-      </c>
-      <c r="O26" t="s">
-        <v>22</v>
+        <v>78.099853889998499</v>
+      </c>
+      <c r="O26">
+        <v>82.310926906617198</v>
       </c>
       <c r="P26">
-        <v>1</v>
+        <v>52.820203721387699</v>
       </c>
       <c r="Q26">
-        <v>78.099853889998499</v>
+        <v>21.6909792336488</v>
       </c>
       <c r="R26">
-        <v>82.310926906617198</v>
+        <v>35.317669917586102</v>
       </c>
       <c r="S26">
-        <v>52.820203721387699</v>
+        <v>11.386161634676901</v>
       </c>
       <c r="T26">
-        <v>21.6909792336488</v>
+        <v>25.297114569108199</v>
       </c>
       <c r="U26">
-        <v>35.317669917586102</v>
-      </c>
-      <c r="V26">
-        <v>11.386161634676901</v>
-      </c>
-      <c r="W26">
-        <v>25.297114569108199</v>
-      </c>
-      <c r="X26">
         <v>4.0207814577115598E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>12</v>
       </c>
@@ -4299,59 +4070,50 @@
         <v>50</v>
       </c>
       <c r="H27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I27">
         <v>3</v>
       </c>
       <c r="J27">
-        <v>3</v>
+        <f>C27*I27*H27/F27/B27</f>
+        <v>0.04</v>
       </c>
       <c r="K27">
-        <f t="shared" si="1"/>
-        <v>0.04</v>
+        <v>64.739999999999995</v>
       </c>
       <c r="L27">
-        <v>64.739999999999995</v>
+        <v>1.0830450542812</v>
       </c>
       <c r="M27">
-        <v>1.0830450542812</v>
+        <v>0</v>
       </c>
       <c r="N27">
-        <v>0</v>
-      </c>
-      <c r="O27" t="s">
-        <v>22</v>
+        <v>80.506947293362003</v>
+      </c>
+      <c r="O27">
+        <v>84.809352309998502</v>
       </c>
       <c r="P27">
-        <v>1</v>
+        <v>55.402323310092598</v>
       </c>
       <c r="Q27">
-        <v>80.506947293362003</v>
+        <v>23.117876243669201</v>
       </c>
       <c r="R27">
-        <v>84.809352309998502</v>
+        <v>41.434218846194099</v>
       </c>
       <c r="S27">
-        <v>55.402323310092598</v>
+        <v>14.281177062235599</v>
       </c>
       <c r="T27">
-        <v>23.117876243669201</v>
+        <v>31.345761025717799</v>
       </c>
       <c r="U27">
-        <v>41.434218846194099</v>
-      </c>
-      <c r="V27">
-        <v>14.281177062235599</v>
-      </c>
-      <c r="W27">
-        <v>31.345761025717799</v>
-      </c>
-      <c r="X27">
         <v>5.0918786039488902E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>13</v>
       </c>
@@ -4374,59 +4136,50 @@
         <v>50</v>
       </c>
       <c r="H28">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I28">
         <v>3</v>
       </c>
       <c r="J28">
-        <v>3</v>
+        <f>C28*I28*H28/F28/B28</f>
+        <v>0.03</v>
       </c>
       <c r="K28">
-        <f t="shared" si="1"/>
-        <v>0.03</v>
+        <v>25.57</v>
       </c>
       <c r="L28">
-        <v>25.57</v>
+        <v>0.23964415554653701</v>
       </c>
       <c r="M28">
-        <v>0.23964415554653701</v>
+        <v>0</v>
       </c>
       <c r="N28">
-        <v>0</v>
-      </c>
-      <c r="O28" t="s">
-        <v>22</v>
+        <v>77.847567232519793</v>
+      </c>
+      <c r="O28">
+        <v>82.0892128062045</v>
       </c>
       <c r="P28">
-        <v>1</v>
+        <v>53.195330076164602</v>
       </c>
       <c r="Q28">
-        <v>77.847567232519793</v>
+        <v>21.2634002652646</v>
       </c>
       <c r="R28">
-        <v>82.0892128062045</v>
+        <v>35.240798295120797</v>
       </c>
       <c r="S28">
-        <v>53.195330076164602</v>
+        <v>11.1522742556091</v>
       </c>
       <c r="T28">
-        <v>21.2634002652646</v>
+        <v>25.230783947643801</v>
       </c>
       <c r="U28">
-        <v>35.240798295120797</v>
-      </c>
-      <c r="V28">
-        <v>11.1522742556091</v>
-      </c>
-      <c r="W28">
-        <v>25.230783947643801</v>
-      </c>
-      <c r="X28">
         <v>3.58190954901261E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>14</v>
       </c>
@@ -4449,59 +4202,50 @@
         <v>50</v>
       </c>
       <c r="H29">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I29">
         <v>3</v>
       </c>
       <c r="J29">
-        <v>3</v>
+        <f>C29*I29*H29/F29/B29</f>
+        <v>2.4E-2</v>
       </c>
       <c r="K29">
-        <f t="shared" si="1"/>
-        <v>2.4E-2</v>
+        <v>21.89</v>
       </c>
       <c r="L29">
-        <v>21.89</v>
+        <v>0.29152830824614201</v>
       </c>
       <c r="M29">
-        <v>0.29152830824614201</v>
+        <v>0</v>
       </c>
       <c r="N29">
-        <v>0</v>
-      </c>
-      <c r="O29" t="s">
-        <v>22</v>
+        <v>78.024600702602498</v>
+      </c>
+      <c r="O29">
+        <v>82.244235959037596</v>
       </c>
       <c r="P29">
-        <v>1</v>
+        <v>52.762399494288204</v>
       </c>
       <c r="Q29">
-        <v>78.024600702602498</v>
+        <v>21.5697285983798</v>
       </c>
       <c r="R29">
-        <v>82.244235959037596</v>
+        <v>35.216738710157998</v>
       </c>
       <c r="S29">
-        <v>52.762399494288204</v>
+        <v>11.3293510604029</v>
       </c>
       <c r="T29">
-        <v>21.5697285983798</v>
+        <v>25.230655375211999</v>
       </c>
       <c r="U29">
-        <v>35.216738710157998</v>
-      </c>
-      <c r="V29">
-        <v>11.3293510604029</v>
-      </c>
-      <c r="W29">
-        <v>25.230655375211999</v>
-      </c>
-      <c r="X29">
         <v>3.8272900123104102E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>15</v>
       </c>
@@ -4524,59 +4268,50 @@
         <v>50</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I30">
         <v>3</v>
       </c>
       <c r="J30">
-        <v>3</v>
+        <f>C30*I30*H30/F30/B30</f>
+        <v>0.02</v>
       </c>
       <c r="K30">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
+        <v>20.190000000000001</v>
       </c>
       <c r="L30">
-        <v>20.190000000000001</v>
+        <v>1.0743562617568401</v>
       </c>
       <c r="M30">
-        <v>1.0743562617568401</v>
+        <v>0</v>
       </c>
       <c r="N30">
-        <v>0</v>
-      </c>
-      <c r="O30" t="s">
-        <v>22</v>
+        <v>80.438248744348797</v>
+      </c>
+      <c r="O30">
+        <v>84.7530288023232</v>
       </c>
       <c r="P30">
-        <v>1</v>
+        <v>55.345025630159498</v>
       </c>
       <c r="Q30">
-        <v>80.438248744348797</v>
+        <v>23.010736874053698</v>
       </c>
       <c r="R30">
-        <v>84.7530288023232</v>
+        <v>41.330384520654299</v>
       </c>
       <c r="S30">
-        <v>55.345025630159498</v>
+        <v>14.1977249008636</v>
       </c>
       <c r="T30">
-        <v>23.010736874053698</v>
+        <v>31.2699135152378</v>
       </c>
       <c r="U30">
-        <v>41.330384520654299</v>
-      </c>
-      <c r="V30">
-        <v>14.1977249008636</v>
-      </c>
-      <c r="W30">
-        <v>31.2699135152378</v>
-      </c>
-      <c r="X30">
         <v>4.9027696449712704E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>16</v>
       </c>
@@ -4599,59 +4334,50 @@
         <v>50</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I31">
         <v>3</v>
       </c>
       <c r="J31">
-        <v>3</v>
+        <f>C31*I31*H31/F31/B31</f>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="K31">
-        <f t="shared" si="1"/>
-        <v>1.4999999999999999E-2</v>
+        <v>7.83</v>
       </c>
       <c r="L31">
-        <v>7.83</v>
+        <v>0.24087727657659699</v>
       </c>
       <c r="M31">
-        <v>0.24087727657659699</v>
+        <v>0</v>
       </c>
       <c r="N31">
-        <v>0</v>
-      </c>
-      <c r="O31" t="s">
-        <v>22</v>
+        <v>77.658877072541301</v>
+      </c>
+      <c r="O31">
+        <v>81.928018126500504</v>
       </c>
       <c r="P31">
-        <v>1</v>
+        <v>53.143461822716702</v>
       </c>
       <c r="Q31">
-        <v>77.658877072541301</v>
+        <v>21.012705280759601</v>
       </c>
       <c r="R31">
-        <v>81.928018126500504</v>
+        <v>35.073117981663003</v>
       </c>
       <c r="S31">
-        <v>53.143461822716702</v>
+        <v>11.0040842507081</v>
       </c>
       <c r="T31">
-        <v>21.012705280759601</v>
+        <v>25.1399156673825</v>
       </c>
       <c r="U31">
-        <v>35.073117981663003</v>
-      </c>
-      <c r="V31">
-        <v>11.0040842507081</v>
-      </c>
-      <c r="W31">
-        <v>25.1399156673825</v>
-      </c>
-      <c r="X31">
         <v>2.9337712692552001E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>17</v>
       </c>
@@ -4674,59 +4400,50 @@
         <v>50</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I32">
         <v>3</v>
       </c>
       <c r="J32">
-        <v>3</v>
+        <f>C32*I32*H32/F32/B32</f>
+        <v>1.2E-2</v>
       </c>
       <c r="K32">
-        <f t="shared" si="1"/>
-        <v>1.2E-2</v>
+        <v>7.25</v>
       </c>
       <c r="L32">
-        <v>7.25</v>
+        <v>0.28800750692021698</v>
       </c>
       <c r="M32">
-        <v>0.28800750692021698</v>
+        <v>0</v>
       </c>
       <c r="N32">
-        <v>0</v>
-      </c>
-      <c r="O32" t="s">
-        <v>22</v>
+        <v>77.867975257105599</v>
+      </c>
+      <c r="O32">
+        <v>82.110520768990298</v>
       </c>
       <c r="P32">
-        <v>1</v>
+        <v>52.719529783863798</v>
       </c>
       <c r="Q32">
-        <v>77.867975257105599</v>
+        <v>21.332175164755601</v>
       </c>
       <c r="R32">
-        <v>82.110520768990298</v>
+        <v>35.085472727058402</v>
       </c>
       <c r="S32">
-        <v>52.719529783863798</v>
+        <v>11.2227621758979</v>
       </c>
       <c r="T32">
-        <v>21.332175164755601</v>
+        <v>25.1652670150179</v>
       </c>
       <c r="U32">
-        <v>35.085472727058402</v>
-      </c>
-      <c r="V32">
-        <v>11.2227621758979</v>
-      </c>
-      <c r="W32">
-        <v>25.1652670150179</v>
-      </c>
-      <c r="X32">
         <v>3.2542798297185999E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>18</v>
       </c>
@@ -4749,59 +4466,50 @@
         <v>50</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I33">
         <v>3</v>
       </c>
       <c r="J33">
-        <v>3</v>
+        <f>C33*I33*H33/F33/B33</f>
+        <v>0.01</v>
       </c>
       <c r="K33">
-        <f t="shared" si="1"/>
-        <v>0.01</v>
+        <v>6.61</v>
       </c>
       <c r="L33">
-        <v>6.61</v>
+        <v>1.0611674356338701</v>
       </c>
       <c r="M33">
-        <v>1.0611674356338701</v>
+        <v>0</v>
       </c>
       <c r="N33">
-        <v>0</v>
-      </c>
-      <c r="O33" t="s">
-        <v>22</v>
+        <v>80.298888920217706</v>
+      </c>
+      <c r="O33">
+        <v>84.641696246691595</v>
       </c>
       <c r="P33">
-        <v>1</v>
+        <v>55.269301123263901</v>
       </c>
       <c r="Q33">
-        <v>80.298888920217706</v>
+        <v>22.7977250105872</v>
       </c>
       <c r="R33">
-        <v>84.641696246691595</v>
+        <v>41.160907099759797</v>
       </c>
       <c r="S33">
-        <v>55.269301123263901</v>
+        <v>14.0306395689227</v>
       </c>
       <c r="T33">
-        <v>22.7977250105872</v>
+        <v>31.154240964576601</v>
       </c>
       <c r="U33">
-        <v>41.160907099759797</v>
-      </c>
-      <c r="V33">
-        <v>14.0306395689227</v>
-      </c>
-      <c r="W33">
-        <v>31.154240964576601</v>
-      </c>
-      <c r="X33">
         <v>4.4257855243472503E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>19</v>
       </c>
@@ -4824,59 +4532,50 @@
         <v>10</v>
       </c>
       <c r="H34">
-        <v>2</v>
+        <v>2.38</v>
       </c>
       <c r="I34">
-        <v>2.38</v>
+        <v>3</v>
       </c>
       <c r="J34">
-        <v>3</v>
+        <f>C34*I34*H34/F34/B34</f>
+        <v>4.7599999999999996E-2</v>
       </c>
       <c r="K34">
-        <f t="shared" si="1"/>
-        <v>4.7599999999999996E-2</v>
+        <v>72.540000000000006</v>
       </c>
       <c r="L34">
-        <v>72.540000000000006</v>
+        <v>0</v>
       </c>
       <c r="M34">
         <v>0</v>
       </c>
       <c r="N34">
-        <v>0</v>
-      </c>
-      <c r="O34" t="s">
-        <v>22</v>
+        <v>78.310226737997993</v>
+      </c>
+      <c r="O34">
+        <v>83.195002958037705</v>
       </c>
       <c r="P34">
-        <v>19</v>
+        <v>54.926561541837401</v>
       </c>
       <c r="Q34">
-        <v>78.310226737997993</v>
+        <v>20.486958237604501</v>
       </c>
       <c r="R34">
-        <v>83.195002958037705</v>
+        <v>33.743617427850097</v>
       </c>
       <c r="S34">
-        <v>54.926561541837401</v>
+        <v>11.458180367545999</v>
       </c>
       <c r="T34">
-        <v>20.486958237604501</v>
+        <v>28.790468807220499</v>
       </c>
       <c r="U34">
-        <v>33.743617427850097</v>
-      </c>
-      <c r="V34">
-        <v>11.458180367545999</v>
-      </c>
-      <c r="W34">
-        <v>28.790468807220499</v>
-      </c>
-      <c r="X34">
         <v>3.73804546143219E-5</v>
       </c>
     </row>
-    <row r="35" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>20</v>
       </c>
@@ -4899,59 +4598,50 @@
         <v>10</v>
       </c>
       <c r="H35">
-        <v>2</v>
+        <v>2.38</v>
       </c>
       <c r="I35">
-        <v>2.38</v>
+        <v>3</v>
       </c>
       <c r="J35">
-        <v>3</v>
+        <f>C35*I35*H35/F35/B35</f>
+        <v>3.8079999999999996E-2</v>
       </c>
       <c r="K35">
-        <f t="shared" si="1"/>
-        <v>3.8079999999999996E-2</v>
+        <v>61.3</v>
       </c>
       <c r="L35">
-        <v>61.3</v>
+        <v>5.3938199684975499E-2</v>
       </c>
       <c r="M35">
-        <v>5.3938199684975499E-2</v>
+        <v>0</v>
       </c>
       <c r="N35">
-        <v>0</v>
-      </c>
-      <c r="O35" t="s">
-        <v>22</v>
+        <v>78.428792739220896</v>
+      </c>
+      <c r="O35">
+        <v>83.288543456311302</v>
       </c>
       <c r="P35">
-        <v>19</v>
+        <v>54.345022214492701</v>
       </c>
       <c r="Q35">
-        <v>78.428792739220896</v>
+        <v>20.760499006902901</v>
       </c>
       <c r="R35">
-        <v>83.288543456311302</v>
+        <v>33.991331459056603</v>
       </c>
       <c r="S35">
-        <v>54.345022214492701</v>
+        <v>11.6870337603319</v>
       </c>
       <c r="T35">
-        <v>20.760499006902901</v>
+        <v>28.650407931896801</v>
       </c>
       <c r="U35">
-        <v>33.991331459056603</v>
-      </c>
-      <c r="V35">
-        <v>11.6870337603319</v>
-      </c>
-      <c r="W35">
-        <v>28.650407931896801</v>
-      </c>
-      <c r="X35">
         <v>3.7585894347103001E-5</v>
       </c>
     </row>
-    <row r="36" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>1</v>
       </c>
@@ -4974,35 +4664,26 @@
         <v>10</v>
       </c>
       <c r="H36">
-        <v>1</v>
+        <v>1.7</v>
       </c>
       <c r="I36">
-        <v>1.7</v>
+        <v>3</v>
       </c>
       <c r="J36">
-        <v>3</v>
+        <f>C36*I36*H36/F36/B36</f>
+        <v>2.7199999999999998E-2</v>
       </c>
       <c r="K36">
-        <f t="shared" si="1"/>
-        <v>2.7199999999999998E-2</v>
+        <v>31.69</v>
       </c>
       <c r="L36">
-        <v>31.69</v>
+        <v>0</v>
       </c>
       <c r="M36">
         <v>0</v>
       </c>
-      <c r="N36">
-        <v>0</v>
-      </c>
-      <c r="O36" t="s">
-        <v>22</v>
-      </c>
-      <c r="P36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:24" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2</v>
       </c>
@@ -5025,32 +4706,179 @@
         <v>10</v>
       </c>
       <c r="H37">
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="I37">
-        <v>1.7</v>
+        <v>3</v>
       </c>
       <c r="J37">
-        <v>3</v>
+        <f>C37*I37*H37/F37/B37</f>
+        <v>2.7199999999999998E-2</v>
       </c>
       <c r="K37">
-        <f t="shared" si="1"/>
-        <v>2.7199999999999998E-2</v>
+        <v>32.35</v>
       </c>
       <c r="L37">
-        <v>32.35</v>
+        <v>0</v>
       </c>
       <c r="M37">
         <v>0</v>
       </c>
-      <c r="N37">
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
+        <v>1</v>
+      </c>
+      <c r="B38" s="11">
+        <v>12.5</v>
+      </c>
+      <c r="C38" s="11">
+        <v>2</v>
+      </c>
+      <c r="D38" s="11">
+        <v>33.5</v>
+      </c>
+      <c r="E38" s="11">
+        <v>33.5</v>
+      </c>
+      <c r="F38" s="11">
+        <v>30</v>
+      </c>
+      <c r="G38" s="11">
+        <v>30</v>
+      </c>
+      <c r="H38" s="11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I38" s="11">
+        <v>3</v>
+      </c>
+      <c r="J38" s="11"/>
+      <c r="K38" s="11">
+        <v>57.67</v>
+      </c>
+      <c r="L38" s="11">
         <v>0</v>
       </c>
-      <c r="O37" t="s">
-        <v>22</v>
-      </c>
-      <c r="P37">
+      <c r="M38" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" s="11">
         <v>2</v>
+      </c>
+      <c r="B39" s="11">
+        <v>12.5</v>
+      </c>
+      <c r="C39" s="11">
+        <v>2</v>
+      </c>
+      <c r="D39" s="11">
+        <v>33.5</v>
+      </c>
+      <c r="E39" s="11">
+        <v>33.5</v>
+      </c>
+      <c r="F39" s="11">
+        <v>30</v>
+      </c>
+      <c r="G39" s="11">
+        <v>30</v>
+      </c>
+      <c r="H39" s="11">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I39" s="11">
+        <v>3</v>
+      </c>
+      <c r="J39" s="11"/>
+      <c r="K39" s="11">
+        <v>67.41</v>
+      </c>
+      <c r="L39" s="11">
+        <v>0</v>
+      </c>
+      <c r="M39" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A40" s="11">
+        <v>3</v>
+      </c>
+      <c r="B40" s="11">
+        <v>12.5</v>
+      </c>
+      <c r="C40" s="11">
+        <v>2</v>
+      </c>
+      <c r="D40" s="11">
+        <v>33.5</v>
+      </c>
+      <c r="E40" s="11">
+        <v>33.5</v>
+      </c>
+      <c r="F40" s="11">
+        <v>30</v>
+      </c>
+      <c r="G40" s="11">
+        <v>30</v>
+      </c>
+      <c r="H40" s="11">
+        <v>2.1749999999999998</v>
+      </c>
+      <c r="I40" s="11">
+        <v>3</v>
+      </c>
+      <c r="J40" s="11"/>
+      <c r="K40" s="11">
+        <v>65.56</v>
+      </c>
+      <c r="L40" s="11">
+        <v>0</v>
+      </c>
+      <c r="M40" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A41" s="11">
+        <v>4</v>
+      </c>
+      <c r="B41" s="11">
+        <v>12.5</v>
+      </c>
+      <c r="C41" s="11">
+        <v>2</v>
+      </c>
+      <c r="D41" s="11">
+        <v>33.5</v>
+      </c>
+      <c r="E41" s="11">
+        <v>33.5</v>
+      </c>
+      <c r="F41" s="11">
+        <v>30</v>
+      </c>
+      <c r="G41" s="11">
+        <v>30</v>
+      </c>
+      <c r="H41" s="11">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I41" s="11">
+        <v>3</v>
+      </c>
+      <c r="J41" s="11"/>
+      <c r="K41" s="11">
+        <v>1.63</v>
+      </c>
+      <c r="L41" s="11">
+        <v>0</v>
+      </c>
+      <c r="M41" s="11">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5060,10 +4888,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S37"/>
+  <dimension ref="A1:S44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I40" sqref="A38:I40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5082,7 +4910,7 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="str">
         <f>data!B1</f>
@@ -5097,26 +4925,26 @@
         <v>time.step</v>
       </c>
       <c r="E1" t="str">
+        <f>data!H1</f>
+        <v>depth</v>
+      </c>
+      <c r="F1" t="str">
         <f>data!I1</f>
-        <v>depth</v>
-      </c>
-      <c r="F1" t="str">
-        <f>data!J1</f>
         <v>n.days</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="I1" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
-        <f>data!L2</f>
+        <f>data!K2</f>
         <v>139.16999999999999</v>
       </c>
       <c r="B2">
@@ -5132,11 +4960,11 @@
         <v>120</v>
       </c>
       <c r="E2">
+        <f>data!H2</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F2">
         <f>data!I2</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F2">
-        <f>data!J2</f>
         <v>7</v>
       </c>
       <c r="G2" s="7">
@@ -5152,12 +4980,12 @@
         <v>140.09412725462218</v>
       </c>
       <c r="K2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
-        <f>data!L3</f>
+        <f>data!K3</f>
         <v>139.04</v>
       </c>
       <c r="B3">
@@ -5173,11 +5001,11 @@
         <v>120</v>
       </c>
       <c r="E3">
+        <f>data!H3</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F3">
         <f>data!I3</f>
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="F3">
-        <f>data!J3</f>
         <v>7</v>
       </c>
       <c r="G3" s="7">
@@ -5195,7 +5023,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
-        <f>data!L4</f>
+        <f>data!K4</f>
         <v>137.76</v>
       </c>
       <c r="B4">
@@ -5211,11 +5039,11 @@
         <v>120</v>
       </c>
       <c r="E4">
+        <f>data!H4</f>
+        <v>2.1749999999999998</v>
+      </c>
+      <c r="F4">
         <f>data!I4</f>
-        <v>2.1749999999999998</v>
-      </c>
-      <c r="F4">
-        <f>data!J4</f>
         <v>7</v>
       </c>
       <c r="G4" s="7">
@@ -5231,13 +5059,13 @@
         <v>139.23305334816868</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <f>data!L5</f>
+        <f>data!K5</f>
         <v>138.04</v>
       </c>
       <c r="B5">
@@ -5253,11 +5081,11 @@
         <v>120</v>
       </c>
       <c r="E5">
+        <f>data!H5</f>
+        <v>2.1749999999999998</v>
+      </c>
+      <c r="F5">
         <f>data!I5</f>
-        <v>2.1749999999999998</v>
-      </c>
-      <c r="F5">
-        <f>data!J5</f>
         <v>7</v>
       </c>
       <c r="G5" s="7">
@@ -5273,7 +5101,7 @@
         <v>139.23305334816868</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="L5" s="1">
         <v>0.97261847018992109</v>
@@ -5281,7 +5109,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
-        <f>data!L6</f>
+        <f>data!K6</f>
         <v>5.27</v>
       </c>
       <c r="B6">
@@ -5297,11 +5125,11 @@
         <v>30</v>
       </c>
       <c r="E6">
+        <f>data!H6</f>
+        <v>2.8</v>
+      </c>
+      <c r="F6">
         <f>data!I6</f>
-        <v>2.8</v>
-      </c>
-      <c r="F6">
-        <f>data!J6</f>
         <v>1</v>
       </c>
       <c r="G6" s="7">
@@ -5317,7 +5145,7 @@
         <v>5.5631328841104395</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="L6" s="1">
         <v>0.94598668855458246</v>
@@ -5325,7 +5153,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
-        <f>data!L7</f>
+        <f>data!K7</f>
         <v>4.05</v>
       </c>
       <c r="B7">
@@ -5341,11 +5169,11 @@
         <v>30</v>
       </c>
       <c r="E7">
+        <f>data!H7</f>
+        <v>2.8</v>
+      </c>
+      <c r="F7">
         <f>data!I7</f>
-        <v>2.8</v>
-      </c>
-      <c r="F7">
-        <f>data!J7</f>
         <v>1</v>
       </c>
       <c r="G7" s="7">
@@ -5361,7 +5189,7 @@
         <v>5.0353517252081419</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="L7" s="1">
         <v>0.93698446998034635</v>
@@ -5369,7 +5197,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
-        <f>data!L8</f>
+        <f>data!K8</f>
         <v>1.7</v>
       </c>
       <c r="B8">
@@ -5385,11 +5213,11 @@
         <v>60</v>
       </c>
       <c r="E8">
+        <f>data!H8</f>
+        <v>2.8</v>
+      </c>
+      <c r="F8">
         <f>data!I8</f>
-        <v>2.8</v>
-      </c>
-      <c r="F8">
-        <f>data!J8</f>
         <v>1</v>
       </c>
       <c r="G8" s="7">
@@ -5405,7 +5233,7 @@
         <v>1.9105327159404573</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="L8" s="1">
         <v>0.38698028584063138</v>
@@ -5413,7 +5241,7 @@
     </row>
     <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
-        <f>data!L9</f>
+        <f>data!K9</f>
         <v>1.52</v>
       </c>
       <c r="B9">
@@ -5429,11 +5257,11 @@
         <v>60</v>
       </c>
       <c r="E9">
+        <f>data!H9</f>
+        <v>2.8</v>
+      </c>
+      <c r="F9">
         <f>data!I9</f>
-        <v>2.8</v>
-      </c>
-      <c r="F9">
-        <f>data!J9</f>
         <v>1</v>
       </c>
       <c r="G9" s="7">
@@ -5449,7 +5277,7 @@
         <v>1.7292781617269739</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="L9" s="2">
         <v>36</v>
@@ -5457,7 +5285,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
-        <f>data!L10</f>
+        <f>data!K10</f>
         <v>0.75</v>
       </c>
       <c r="B10">
@@ -5473,11 +5301,11 @@
         <v>120</v>
       </c>
       <c r="E10">
+        <f>data!H10</f>
+        <v>2.8</v>
+      </c>
+      <c r="F10">
         <f>data!I10</f>
-        <v>2.8</v>
-      </c>
-      <c r="F10">
-        <f>data!J10</f>
         <v>1</v>
       </c>
       <c r="G10" s="7">
@@ -5495,7 +5323,7 @@
     </row>
     <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
-        <f>data!L11</f>
+        <f>data!K11</f>
         <v>2.52</v>
       </c>
       <c r="B11">
@@ -5511,11 +5339,11 @@
         <v>30</v>
       </c>
       <c r="E11">
+        <f>data!H11</f>
+        <v>0.5</v>
+      </c>
+      <c r="F11">
         <f>data!I11</f>
-        <v>0.5</v>
-      </c>
-      <c r="F11">
-        <f>data!J11</f>
         <v>1</v>
       </c>
       <c r="G11" s="7">
@@ -5531,12 +5359,12 @@
         <v>3.1548725107447679</v>
       </c>
       <c r="K11" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
-        <f>data!L12</f>
+        <f>data!K12</f>
         <v>2.44</v>
       </c>
       <c r="B12">
@@ -5552,11 +5380,11 @@
         <v>30</v>
       </c>
       <c r="E12">
+        <f>data!H12</f>
+        <v>0.5</v>
+      </c>
+      <c r="F12">
         <f>data!I12</f>
-        <v>0.5</v>
-      </c>
-      <c r="F12">
-        <f>data!J12</f>
         <v>1</v>
       </c>
       <c r="G12" s="7">
@@ -5573,24 +5401,24 @@
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="M12" s="3" t="s">
+      <c r="P12" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <f>data!L13</f>
+        <f>data!K13</f>
         <v>3.69</v>
       </c>
       <c r="B13">
@@ -5606,11 +5434,11 @@
         <v>30</v>
       </c>
       <c r="E13">
+        <f>data!H13</f>
+        <v>2</v>
+      </c>
+      <c r="F13">
         <f>data!I13</f>
-        <v>2</v>
-      </c>
-      <c r="F13">
-        <f>data!J13</f>
         <v>1</v>
       </c>
       <c r="G13" s="7">
@@ -5626,7 +5454,7 @@
         <v>4.5670606967711276</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="L13" s="1">
         <v>5</v>
@@ -5646,7 +5474,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <f>data!L14</f>
+        <f>data!K14</f>
         <v>3.34</v>
       </c>
       <c r="B14">
@@ -5662,11 +5490,11 @@
         <v>30</v>
       </c>
       <c r="E14">
+        <f>data!H14</f>
+        <v>2</v>
+      </c>
+      <c r="F14">
         <f>data!I14</f>
-        <v>2</v>
-      </c>
-      <c r="F14">
-        <f>data!J14</f>
         <v>1</v>
       </c>
       <c r="G14" s="7">
@@ -5682,7 +5510,7 @@
         <v>4.1337781134620588</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="L14" s="1">
         <v>30</v>
@@ -5698,7 +5526,7 @@
     </row>
     <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
-        <f>data!L15</f>
+        <f>data!K15</f>
         <v>1.36</v>
       </c>
       <c r="B15">
@@ -5714,11 +5542,11 @@
         <v>60</v>
       </c>
       <c r="E15">
+        <f>data!H15</f>
+        <v>2</v>
+      </c>
+      <c r="F15">
         <f>data!I15</f>
-        <v>2</v>
-      </c>
-      <c r="F15">
-        <f>data!J15</f>
         <v>1</v>
       </c>
       <c r="G15" s="7">
@@ -5734,7 +5562,7 @@
         <v>1.4196530068094455</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="L15" s="2">
         <v>35</v>
@@ -5748,7 +5576,7 @@
     </row>
     <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
-        <f>data!L16</f>
+        <f>data!K16</f>
         <v>88.24</v>
       </c>
       <c r="B16">
@@ -5764,11 +5592,11 @@
         <v>15</v>
       </c>
       <c r="E16">
+        <f>data!H16</f>
+        <v>3</v>
+      </c>
+      <c r="F16">
         <f>data!I16</f>
-        <v>3</v>
-      </c>
-      <c r="F16">
-        <f>data!J16</f>
         <v>3</v>
       </c>
       <c r="G16" s="7">
@@ -5786,7 +5614,7 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <f>data!L17</f>
+        <f>data!K17</f>
         <v>72.930000000000007</v>
       </c>
       <c r="B17">
@@ -5802,11 +5630,11 @@
         <v>15</v>
       </c>
       <c r="E17">
+        <f>data!H17</f>
+        <v>3</v>
+      </c>
+      <c r="F17">
         <f>data!I17</f>
-        <v>3</v>
-      </c>
-      <c r="F17">
-        <f>data!J17</f>
         <v>3</v>
       </c>
       <c r="G17" s="7">
@@ -5823,33 +5651,33 @@
       </c>
       <c r="K17" s="3"/>
       <c r="L17" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="P17" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="M17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="N17" s="3" t="s">
+      <c r="Q17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="O17" s="3" t="s">
+      <c r="R17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="P17" s="3" t="s">
+      <c r="S17" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="Q17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <f>data!L18</f>
+        <f>data!K18</f>
         <v>65.73</v>
       </c>
       <c r="B18">
@@ -5865,11 +5693,11 @@
         <v>15</v>
       </c>
       <c r="E18">
+        <f>data!H18</f>
+        <v>3</v>
+      </c>
+      <c r="F18">
         <f>data!I18</f>
-        <v>3</v>
-      </c>
-      <c r="F18">
-        <f>data!J18</f>
         <v>3</v>
       </c>
       <c r="G18" s="7">
@@ -5885,7 +5713,7 @@
         <v>45.827083745528483</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L18" s="1">
         <v>1.5516343684670519</v>
@@ -5914,7 +5742,7 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <f>data!L19</f>
+        <f>data!K19</f>
         <v>24.57</v>
       </c>
       <c r="B19">
@@ -5930,11 +5758,11 @@
         <v>30</v>
       </c>
       <c r="E19">
+        <f>data!H19</f>
+        <v>3</v>
+      </c>
+      <c r="F19">
         <f>data!I19</f>
-        <v>3</v>
-      </c>
-      <c r="F19">
-        <f>data!J19</f>
         <v>3</v>
       </c>
       <c r="G19" s="7">
@@ -5979,7 +5807,7 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <f>data!L20</f>
+        <f>data!K20</f>
         <v>22.46</v>
       </c>
       <c r="B20">
@@ -5995,11 +5823,11 @@
         <v>30</v>
       </c>
       <c r="E20">
+        <f>data!H20</f>
+        <v>3</v>
+      </c>
+      <c r="F20">
         <f>data!I20</f>
-        <v>3</v>
-      </c>
-      <c r="F20">
-        <f>data!J20</f>
         <v>3</v>
       </c>
       <c r="G20" s="7">
@@ -6044,7 +5872,7 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <f>data!L21</f>
+        <f>data!K21</f>
         <v>20.260000000000002</v>
       </c>
       <c r="B21">
@@ -6060,11 +5888,11 @@
         <v>30</v>
       </c>
       <c r="E21">
+        <f>data!H21</f>
+        <v>3</v>
+      </c>
+      <c r="F21">
         <f>data!I21</f>
-        <v>3</v>
-      </c>
-      <c r="F21">
-        <f>data!J21</f>
         <v>3</v>
       </c>
       <c r="G21" s="7">
@@ -6109,7 +5937,7 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <f>data!L22</f>
+        <f>data!K22</f>
         <v>8.2899999999999991</v>
       </c>
       <c r="B22">
@@ -6125,11 +5953,11 @@
         <v>60</v>
       </c>
       <c r="E22">
+        <f>data!H22</f>
+        <v>3</v>
+      </c>
+      <c r="F22">
         <f>data!I22</f>
-        <v>3</v>
-      </c>
-      <c r="F22">
-        <f>data!J22</f>
         <v>3</v>
       </c>
       <c r="G22" s="7">
@@ -6145,7 +5973,7 @@
         <v>11.257813061630124</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="L22" s="1">
         <v>0.24661449191347981</v>
@@ -6174,7 +6002,7 @@
     </row>
     <row r="23" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
-        <f>data!L23</f>
+        <f>data!K23</f>
         <v>7.37</v>
       </c>
       <c r="B23">
@@ -6190,11 +6018,11 @@
         <v>60</v>
       </c>
       <c r="E23">
+        <f>data!H23</f>
+        <v>3</v>
+      </c>
+      <c r="F23">
         <f>data!I23</f>
-        <v>3</v>
-      </c>
-      <c r="F23">
-        <f>data!J23</f>
         <v>3</v>
       </c>
       <c r="G23" s="7">
@@ -6210,7 +6038,7 @@
         <v>10.189770692672285</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="L23" s="2">
         <v>0.86217868577260059</v>
@@ -6239,7 +6067,7 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <f>data!L24</f>
+        <f>data!K24</f>
         <v>6.87</v>
       </c>
       <c r="B24">
@@ -6255,11 +6083,11 @@
         <v>60</v>
       </c>
       <c r="E24">
+        <f>data!H24</f>
+        <v>3</v>
+      </c>
+      <c r="F24">
         <f>data!I24</f>
-        <v>3</v>
-      </c>
-      <c r="F24">
-        <f>data!J24</f>
         <v>3</v>
       </c>
       <c r="G24" s="7">
@@ -6277,7 +6105,7 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <f>data!L25</f>
+        <f>data!K25</f>
         <v>88.38</v>
       </c>
       <c r="B25">
@@ -6293,11 +6121,11 @@
         <v>15</v>
       </c>
       <c r="E25">
+        <f>data!H25</f>
+        <v>3</v>
+      </c>
+      <c r="F25">
         <f>data!I25</f>
-        <v>3</v>
-      </c>
-      <c r="F25">
-        <f>data!J25</f>
         <v>3</v>
       </c>
       <c r="G25" s="7">
@@ -6315,7 +6143,7 @@
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
-        <f>data!L26</f>
+        <f>data!K26</f>
         <v>73.42</v>
       </c>
       <c r="B26">
@@ -6331,11 +6159,11 @@
         <v>15</v>
       </c>
       <c r="E26">
+        <f>data!H26</f>
+        <v>3</v>
+      </c>
+      <c r="F26">
         <f>data!I26</f>
-        <v>3</v>
-      </c>
-      <c r="F26">
-        <f>data!J26</f>
         <v>3</v>
       </c>
       <c r="G26" s="7">
@@ -6353,7 +6181,7 @@
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
-        <f>data!L27</f>
+        <f>data!K27</f>
         <v>64.739999999999995</v>
       </c>
       <c r="B27">
@@ -6369,11 +6197,11 @@
         <v>15</v>
       </c>
       <c r="E27">
+        <f>data!H27</f>
+        <v>3</v>
+      </c>
+      <c r="F27">
         <f>data!I27</f>
-        <v>3</v>
-      </c>
-      <c r="F27">
-        <f>data!J27</f>
         <v>3</v>
       </c>
       <c r="G27" s="7">
@@ -6391,7 +6219,7 @@
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
-        <f>data!L28</f>
+        <f>data!K28</f>
         <v>25.57</v>
       </c>
       <c r="B28">
@@ -6407,11 +6235,11 @@
         <v>30</v>
       </c>
       <c r="E28">
+        <f>data!H28</f>
+        <v>3</v>
+      </c>
+      <c r="F28">
         <f>data!I28</f>
-        <v>3</v>
-      </c>
-      <c r="F28">
-        <f>data!J28</f>
         <v>3</v>
       </c>
       <c r="G28" s="7">
@@ -6429,7 +6257,7 @@
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
-        <f>data!L29</f>
+        <f>data!K29</f>
         <v>21.89</v>
       </c>
       <c r="B29">
@@ -6445,11 +6273,11 @@
         <v>30</v>
       </c>
       <c r="E29">
+        <f>data!H29</f>
+        <v>3</v>
+      </c>
+      <c r="F29">
         <f>data!I29</f>
-        <v>3</v>
-      </c>
-      <c r="F29">
-        <f>data!J29</f>
         <v>3</v>
       </c>
       <c r="G29" s="7">
@@ -6467,7 +6295,7 @@
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
-        <f>data!L30</f>
+        <f>data!K30</f>
         <v>20.190000000000001</v>
       </c>
       <c r="B30">
@@ -6483,11 +6311,11 @@
         <v>30</v>
       </c>
       <c r="E30">
+        <f>data!H30</f>
+        <v>3</v>
+      </c>
+      <c r="F30">
         <f>data!I30</f>
-        <v>3</v>
-      </c>
-      <c r="F30">
-        <f>data!J30</f>
         <v>3</v>
       </c>
       <c r="G30" s="7">
@@ -6505,7 +6333,7 @@
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
-        <f>data!L31</f>
+        <f>data!K31</f>
         <v>7.83</v>
       </c>
       <c r="B31">
@@ -6521,11 +6349,11 @@
         <v>60</v>
       </c>
       <c r="E31">
+        <f>data!H31</f>
+        <v>3</v>
+      </c>
+      <c r="F31">
         <f>data!I31</f>
-        <v>3</v>
-      </c>
-      <c r="F31">
-        <f>data!J31</f>
         <v>3</v>
       </c>
       <c r="G31" s="7">
@@ -6543,7 +6371,7 @@
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
-        <f>data!L32</f>
+        <f>data!K32</f>
         <v>7.25</v>
       </c>
       <c r="B32">
@@ -6559,11 +6387,11 @@
         <v>60</v>
       </c>
       <c r="E32">
+        <f>data!H32</f>
+        <v>3</v>
+      </c>
+      <c r="F32">
         <f>data!I32</f>
-        <v>3</v>
-      </c>
-      <c r="F32">
-        <f>data!J32</f>
         <v>3</v>
       </c>
       <c r="G32" s="7">
@@ -6581,7 +6409,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
-        <f>data!L33</f>
+        <f>data!K33</f>
         <v>6.61</v>
       </c>
       <c r="B33">
@@ -6597,11 +6425,11 @@
         <v>60</v>
       </c>
       <c r="E33">
+        <f>data!H33</f>
+        <v>3</v>
+      </c>
+      <c r="F33">
         <f>data!I33</f>
-        <v>3</v>
-      </c>
-      <c r="F33">
-        <f>data!J33</f>
         <v>3</v>
       </c>
       <c r="G33" s="7">
@@ -6619,7 +6447,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
-        <f>data!L34</f>
+        <f>data!K34</f>
         <v>72.540000000000006</v>
       </c>
       <c r="B34">
@@ -6635,11 +6463,11 @@
         <v>15</v>
       </c>
       <c r="E34">
+        <f>data!H34</f>
+        <v>2.38</v>
+      </c>
+      <c r="F34">
         <f>data!I34</f>
-        <v>2.38</v>
-      </c>
-      <c r="F34">
-        <f>data!J34</f>
         <v>3</v>
       </c>
       <c r="G34" s="7">
@@ -6657,7 +6485,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
-        <f>data!L35</f>
+        <f>data!K35</f>
         <v>61.3</v>
       </c>
       <c r="B35">
@@ -6673,11 +6501,11 @@
         <v>15</v>
       </c>
       <c r="E35">
+        <f>data!H35</f>
+        <v>2.38</v>
+      </c>
+      <c r="F35">
         <f>data!I35</f>
-        <v>2.38</v>
-      </c>
-      <c r="F35">
-        <f>data!J35</f>
         <v>3</v>
       </c>
       <c r="G35" s="7">
@@ -6695,7 +6523,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
-        <f>data!L36</f>
+        <f>data!K36</f>
         <v>31.69</v>
       </c>
       <c r="B36">
@@ -6711,11 +6539,11 @@
         <v>30</v>
       </c>
       <c r="E36">
+        <f>data!H36</f>
+        <v>1.7</v>
+      </c>
+      <c r="F36">
         <f>data!I36</f>
-        <v>1.7</v>
-      </c>
-      <c r="F36">
-        <f>data!J36</f>
         <v>3</v>
       </c>
       <c r="G36" s="7">
@@ -6733,7 +6561,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
-        <f>data!L37</f>
+        <f>data!K37</f>
         <v>32.35</v>
       </c>
       <c r="B37">
@@ -6749,11 +6577,11 @@
         <v>30</v>
       </c>
       <c r="E37">
+        <f>data!H37</f>
+        <v>1.7</v>
+      </c>
+      <c r="F37">
         <f>data!I37</f>
-        <v>1.7</v>
-      </c>
-      <c r="F37">
-        <f>data!J37</f>
         <v>3</v>
       </c>
       <c r="G37" s="7">
@@ -6768,9 +6596,157 @@
         <f t="shared" si="1"/>
         <v>23.31003734379734</v>
       </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <f>data!K38</f>
+        <v>57.67</v>
+      </c>
+      <c r="B38">
+        <f>data!B38</f>
+        <v>12.5</v>
+      </c>
+      <c r="C38">
+        <f>data!C38</f>
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <f>data!F38</f>
+        <v>30</v>
+      </c>
+      <c r="E38">
+        <f>data!H38</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F38">
+        <f>data!I38</f>
+        <v>3</v>
+      </c>
+      <c r="G38" s="7">
+        <f>regression!$L$18+regression!$L$19*B38+$L$20*C38+$L$21*D38+$L$22*E38+$L$23*F38</f>
+        <v>3.2721913010536303</v>
+      </c>
+      <c r="H38" s="9">
+        <f t="shared" ref="H38:H42" si="2">LN(A38)</f>
+        <v>4.0547371076273215</v>
+      </c>
+      <c r="I38" s="10">
+        <f t="shared" ref="I38:I42" si="3">EXP(G38)</f>
+        <v>26.369058625957333</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
+        <f>data!K39</f>
+        <v>67.41</v>
+      </c>
+      <c r="B39">
+        <f>data!B39</f>
+        <v>12.5</v>
+      </c>
+      <c r="C39">
+        <f>data!C39</f>
+        <v>2</v>
+      </c>
+      <c r="D39">
+        <f>data!F39</f>
+        <v>30</v>
+      </c>
+      <c r="E39">
+        <f>data!H39</f>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F39">
+        <f>data!I39</f>
+        <v>3</v>
+      </c>
+      <c r="G39" s="7">
+        <f>regression!$L$18+regression!$L$19*B39+$L$20*C39+$L$21*D39+$L$22*E39+$L$23*F39</f>
+        <v>3.2721913010536303</v>
+      </c>
+      <c r="H39" s="9">
+        <f t="shared" si="2"/>
+        <v>4.2107933748653474</v>
+      </c>
+      <c r="I39" s="10">
+        <f t="shared" si="3"/>
+        <v>26.369058625957333</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="8">
+        <f>data!K40</f>
+        <v>65.56</v>
+      </c>
+      <c r="B40">
+        <f>data!B40</f>
+        <v>12.5</v>
+      </c>
+      <c r="C40">
+        <f>data!C40</f>
+        <v>2</v>
+      </c>
+      <c r="D40">
+        <f>data!F40</f>
+        <v>30</v>
+      </c>
+      <c r="E40">
+        <f>data!H40</f>
+        <v>2.1749999999999998</v>
+      </c>
+      <c r="F40">
+        <f>data!I40</f>
+        <v>3</v>
+      </c>
+      <c r="G40" s="7">
+        <f>regression!$L$18+regression!$L$19*B40+$L$20*C40+$L$21*D40+$L$22*E40+$L$23*F40</f>
+        <v>3.2660259387557931</v>
+      </c>
+      <c r="H40" s="9">
+        <f t="shared" si="2"/>
+        <v>4.1829657538756289</v>
+      </c>
+      <c r="I40" s="10">
+        <f t="shared" si="3"/>
+        <v>26.206983963974629</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="8"/>
+      <c r="G41" s="7"/>
+      <c r="H41" s="9"/>
+      <c r="I41" s="10"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
+      <c r="G42" s="7"/>
+      <c r="H42" s="9"/>
+      <c r="I42" s="10"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="8"/>
+      <c r="H43" s="9"/>
+      <c r="I43" s="10"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="8"/>
+      <c r="H44" s="9"/>
+      <c r="I44" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>